<commit_message>
upload final excel sheet for cluster analysis
in-class example to cluster grad program outcomes
</commit_message>
<xml_diff>
--- a/2020spring_inclass_excel_work/tabula-Career-Outcome-ADA-Tables-Final_decision_analytics.xlsx
+++ b/2020spring_inclass_excel_work/tabula-Career-Outcome-ADA-Tables-Final_decision_analytics.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10" conformance="strict">
+<workbook xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2" conformance="strict">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10210"/>
   <workbookPr dateCompatibility="0" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/melanieshimano/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{BB215DED-A0EA-0849-9FB1-A03BBC9916B3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{A95AD081-3968-374D-ADA7-EDF14A3A188E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4440" yWindow="460" windowWidth="32120" windowHeight="20720" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="sector_grad" sheetId="1" r:id="rId1"/>
@@ -20,6 +20,44 @@
     <sheet name="career_5yrs" sheetId="5" r:id="rId5"/>
     <sheet name="sector_10yrs" sheetId="3" r:id="rId6"/>
   </sheets>
+  <definedNames>
+    <definedName name="cluster">sector_5yrs!$A$12:$Q$35</definedName>
+    <definedName name="solver_adj" localSheetId="1" hidden="1">sector_5yrs!$D$3:$D$5</definedName>
+    <definedName name="solver_cvg" localSheetId="1" hidden="1">0.0001</definedName>
+    <definedName name="solver_drv" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_eng" localSheetId="1" hidden="1">3</definedName>
+    <definedName name="solver_itr" localSheetId="1" hidden="1">2147483647</definedName>
+    <definedName name="solver_lhs1" localSheetId="1" hidden="1">sector_5yrs!$D$3:$D$5</definedName>
+    <definedName name="solver_lhs2" localSheetId="1" hidden="1">sector_5yrs!$D$3:$D$5</definedName>
+    <definedName name="solver_lhs3" localSheetId="1" hidden="1">sector_5yrs!$D$3:$D$5</definedName>
+    <definedName name="solver_lin" localSheetId="1" hidden="1">2</definedName>
+    <definedName name="solver_mip" localSheetId="1" hidden="1">2147483647</definedName>
+    <definedName name="solver_mni" localSheetId="1" hidden="1">30</definedName>
+    <definedName name="solver_mrt" localSheetId="1" hidden="1">0.075</definedName>
+    <definedName name="solver_msl" localSheetId="1" hidden="1">2</definedName>
+    <definedName name="solver_neg" localSheetId="1" hidden="1">2</definedName>
+    <definedName name="solver_nod" localSheetId="1" hidden="1">2147483647</definedName>
+    <definedName name="solver_num" localSheetId="1" hidden="1">3</definedName>
+    <definedName name="solver_opt" localSheetId="1" hidden="1">sector_5yrs!$U$5</definedName>
+    <definedName name="solver_pre" localSheetId="1" hidden="1">0.000001</definedName>
+    <definedName name="solver_rbv" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_rel1" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_rel2" localSheetId="1" hidden="1">4</definedName>
+    <definedName name="solver_rel3" localSheetId="1" hidden="1">3</definedName>
+    <definedName name="solver_rhs1" localSheetId="1" hidden="1">21</definedName>
+    <definedName name="solver_rhs2" localSheetId="1" hidden="1">integer</definedName>
+    <definedName name="solver_rhs3" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_rlx" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_rsd" localSheetId="1" hidden="1">0</definedName>
+    <definedName name="solver_scl" localSheetId="1" hidden="1">2</definedName>
+    <definedName name="solver_sho" localSheetId="1" hidden="1">2</definedName>
+    <definedName name="solver_ssz" localSheetId="1" hidden="1">100</definedName>
+    <definedName name="solver_tim" localSheetId="1" hidden="1">2147483647</definedName>
+    <definedName name="solver_tol" localSheetId="1" hidden="1">0.01</definedName>
+    <definedName name="solver_typ" localSheetId="1" hidden="1">2</definedName>
+    <definedName name="solver_val" localSheetId="1" hidden="1">0</definedName>
+    <definedName name="solver_ver" localSheetId="1" hidden="1">2</definedName>
+  </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
@@ -30,7 +68,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="602" uniqueCount="319">
+<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="613" uniqueCount="324">
   <si>
     <t>Sector Upon Graduation (N=1,453)</t>
   </si>
@@ -959,40 +997,55 @@
     <t>standard_deviation</t>
   </si>
   <si>
-    <t>z_aca_n</t>
-  </si>
-  <si>
     <t>z_aca_%</t>
   </si>
   <si>
-    <t>z_forprof_n</t>
-  </si>
-  <si>
     <t>z_forprof_%</t>
   </si>
   <si>
-    <t>z_gov_n</t>
-  </si>
-  <si>
     <t>z_gov_%</t>
   </si>
   <si>
-    <t>z_nonprof_n</t>
-  </si>
-  <si>
     <t>z_nonprof_%</t>
   </si>
   <si>
-    <t>z_not_found_n</t>
-  </si>
-  <si>
     <t>z_not_found_%</t>
+  </si>
+  <si>
+    <t>cluster_number</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>cluster_name</t>
+  </si>
+  <si>
+    <t>distsq_1</t>
+  </si>
+  <si>
+    <t>distsq_2</t>
+  </si>
+  <si>
+    <t>distsq_3</t>
+  </si>
+  <si>
+    <t>min_distsq</t>
+  </si>
+  <si>
+    <t>cluster_match</t>
+  </si>
+  <si>
+    <t>sum_min_distsq</t>
+  </si>
+  <si>
+    <t>name_of_cluster_nod</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18">
     <font>
       <sz val="12"/>
@@ -1129,7 +1182,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="37">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1309,6 +1362,30 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="11">
     <border>
@@ -1479,10 +1556,19 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1837,7 +1923,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L26"/>
   <sheetViews>
     <sheetView zoomScale="165" zoomScaleNormal="165" workbookViewId="0">
@@ -2650,1790 +2736,2081 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A4:U30"/>
+<worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:X35"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="U20" sqref="U20"/>
+    <sheetView tabSelected="1" zoomScale="137" zoomScaleNormal="137" workbookViewId="0">
+      <selection activeCell="Z12" sqref="Z12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="44.6640625" customWidth="1"/>
-    <col min="2" max="2" width="6.5" customWidth="1"/>
-    <col min="12" max="12" width="7.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="44.6640625" customWidth="1"/>
+    <col min="3" max="3" width="6.5" customWidth="1"/>
+    <col min="5" max="5" width="29.6640625" customWidth="1"/>
     <col min="13" max="13" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="11" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="7.83203125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="11.83203125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="13.83203125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="14.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="1:21">
-      <c r="A4" s="1" t="s">
+    <row r="1" spans="1:24">
+      <c r="F1">
+        <v>13</v>
+      </c>
+      <c r="G1">
+        <v>14</v>
+      </c>
+      <c r="H1">
+        <v>15</v>
+      </c>
+      <c r="I1">
+        <v>16</v>
+      </c>
+      <c r="J1">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:24">
+      <c r="C2" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>315</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>316</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>309</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>310</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>312</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="3" spans="1:24">
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>20</v>
+      </c>
+      <c r="E3" t="str">
+        <f>VLOOKUP(D3,cluster,2,)</f>
+        <v>Pathobiology</v>
+      </c>
+      <c r="F3">
+        <f>VLOOKUP($D3,cluster,13,FALSE())</f>
+        <v>-0.35548787066454079</v>
+      </c>
+      <c r="G3">
+        <f>VLOOKUP($D3,cluster,G$1,FALSE())</f>
+        <v>1.4580134416999975</v>
+      </c>
+      <c r="H3">
+        <f>VLOOKUP($D3,cluster,H$1,FALSE())</f>
+        <v>-0.63677081779374334</v>
+      </c>
+      <c r="I3">
+        <f>VLOOKUP($D3,cluster,I$1,FALSE())</f>
+        <v>4.8917450524135916E-2</v>
+      </c>
+      <c r="J3">
+        <f>VLOOKUP($D3,cluster,J$1,FALSE())</f>
+        <v>-0.61690351932569254</v>
+      </c>
+    </row>
+    <row r="4" spans="1:24">
+      <c r="C4">
+        <v>2</v>
+      </c>
+      <c r="D4">
+        <v>12</v>
+      </c>
+      <c r="E4" t="str">
+        <f>VLOOKUP(D4,cluster,2,)</f>
+        <v>Clinical Investigation</v>
+      </c>
+      <c r="F4">
+        <f>VLOOKUP($D4,cluster,F$1,FALSE())</f>
+        <v>-0.44765139268868109</v>
+      </c>
+      <c r="G4">
+        <f>VLOOKUP($D4,cluster,G$1,FALSE())</f>
+        <v>-1.311081854551936</v>
+      </c>
+      <c r="H4">
+        <f>VLOOKUP($D4,cluster,H$1,FALSE())</f>
+        <v>-0.94417741948727474</v>
+      </c>
+      <c r="I4">
+        <f>VLOOKUP($D4,cluster,I$1,FALSE())</f>
+        <v>-1.3207711641516702</v>
+      </c>
+      <c r="J4">
+        <f>VLOOKUP($D4,cluster,J$1,FALSE())</f>
+        <v>1.6597027737507128</v>
+      </c>
+      <c r="U4" s="1" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="5" spans="1:24">
+      <c r="C5">
+        <v>3</v>
+      </c>
+      <c r="D5">
+        <v>3</v>
+      </c>
+      <c r="E5" t="str">
+        <f>VLOOKUP(D5,cluster,2,)</f>
+        <v>Biological Chemistry</v>
+      </c>
+      <c r="F5">
+        <f>VLOOKUP($D5,cluster,F$1,FALSE())</f>
+        <v>0.56614734957686197</v>
+      </c>
+      <c r="G5">
+        <f>VLOOKUP($D5,cluster,G$1,FALSE())</f>
+        <v>-0.2825607445155035</v>
+      </c>
+      <c r="H5">
+        <f>VLOOKUP($D5,cluster,H$1,FALSE())</f>
+        <v>0.43915228813361629</v>
+      </c>
+      <c r="I5">
+        <f>VLOOKUP($D5,cluster,I$1,FALSE())</f>
+        <v>0.39133960419308744</v>
+      </c>
+      <c r="J5">
+        <f>VLOOKUP($D5,cluster,J$1,FALSE())</f>
+        <v>-0.3458789606261205</v>
+      </c>
+      <c r="U5">
+        <f>SUM(U15:U35)</f>
+        <v>52.182957959018694</v>
+      </c>
+    </row>
+    <row r="8" spans="1:24" s="4" customFormat="1"/>
+    <row r="9" spans="1:24">
+      <c r="B9" s="1" t="s">
         <v>307</v>
       </c>
-      <c r="B4">
-        <f>AVERAGE(B10:B30)</f>
+      <c r="C9">
+        <f>AVERAGE(C15:C35)</f>
         <v>24.238095238095237</v>
       </c>
-      <c r="C4">
-        <f t="shared" ref="C4:K4" si="0">AVERAGE(C10:C30)</f>
+      <c r="D9">
+        <f t="shared" ref="D9:L9" si="0">AVERAGE(D15:D35)</f>
         <v>33.857142857142854</v>
       </c>
-      <c r="D4">
+      <c r="E9">
         <f t="shared" si="0"/>
         <v>12.380952380952381</v>
       </c>
-      <c r="E4">
+      <c r="F9">
         <f t="shared" si="0"/>
         <v>16.571428571428573</v>
       </c>
-      <c r="F4">
+      <c r="G9">
         <f t="shared" si="0"/>
         <v>7.1904761904761907</v>
       </c>
-      <c r="G4">
+      <c r="H9">
         <f t="shared" si="0"/>
         <v>8.1428571428571423</v>
       </c>
-      <c r="H4">
+      <c r="I9">
         <f t="shared" si="0"/>
         <v>3.3333333333333335</v>
       </c>
-      <c r="I4">
+      <c r="J9">
         <f t="shared" si="0"/>
         <v>3.8571428571428572</v>
       </c>
-      <c r="J4">
+      <c r="K9">
         <f t="shared" si="0"/>
         <v>22.047619047619047</v>
       </c>
-      <c r="K4" s="2">
+      <c r="L9" s="2">
         <f t="shared" si="0"/>
         <v>37.38095238095238</v>
       </c>
-    </row>
-    <row r="5" spans="1:21">
-      <c r="A5" s="1" t="s">
+      <c r="Q9" s="2"/>
+    </row>
+    <row r="10" spans="1:24">
+      <c r="B10" s="1" t="s">
         <v>308</v>
       </c>
-      <c r="B5">
-        <f>STDEV(B10:B30)</f>
+      <c r="C10">
+        <f>STDEV(C15:C35)</f>
         <v>19.333661737769081</v>
       </c>
-      <c r="C5">
-        <f t="shared" ref="C5:K5" si="1">STDEV(C10:C30)</f>
+      <c r="D10">
+        <f t="shared" ref="D10:L10" si="1">STDEV(D15:D35)</f>
         <v>10.850279785727711</v>
       </c>
-      <c r="D5">
+      <c r="E10">
         <f t="shared" si="1"/>
         <v>11.482491848358485</v>
       </c>
-      <c r="E5">
+      <c r="F10">
         <f t="shared" si="1"/>
         <v>12.639507223667497</v>
       </c>
-      <c r="F5">
+      <c r="G10">
         <f t="shared" si="1"/>
         <v>7.749961597447097</v>
       </c>
-      <c r="G5">
+      <c r="H10">
         <f t="shared" si="1"/>
         <v>6.5060411486995253</v>
       </c>
-      <c r="H5">
+      <c r="I10">
         <f t="shared" si="1"/>
         <v>3.4253953543107007</v>
       </c>
-      <c r="I5">
+      <c r="J10">
         <f t="shared" si="1"/>
         <v>2.9203717962909157</v>
       </c>
-      <c r="J5">
+      <c r="K10">
         <f t="shared" si="1"/>
         <v>16.329348396296133</v>
       </c>
-      <c r="K5" s="2">
+      <c r="L10" s="2">
         <f t="shared" si="1"/>
         <v>18.448512651366212</v>
       </c>
-    </row>
-    <row r="6" spans="1:21">
-      <c r="K6" s="2"/>
-    </row>
-    <row r="7" spans="1:21">
-      <c r="B7" t="s">
+      <c r="Q10" s="2"/>
+    </row>
+    <row r="11" spans="1:24">
+      <c r="A11">
+        <v>1</v>
+      </c>
+      <c r="B11">
         <v>2</v>
       </c>
-      <c r="D7" t="s">
+      <c r="C11">
         <v>3</v>
       </c>
-      <c r="F7" t="s">
+      <c r="D11">
         <v>4</v>
       </c>
-      <c r="H7" t="s">
+      <c r="E11">
         <v>5</v>
       </c>
-      <c r="J7" t="s">
+      <c r="F11">
+        <v>6</v>
+      </c>
+      <c r="G11">
+        <v>7</v>
+      </c>
+      <c r="H11">
+        <v>8</v>
+      </c>
+      <c r="I11">
+        <v>9</v>
+      </c>
+      <c r="J11">
+        <v>10</v>
+      </c>
+      <c r="K11">
+        <v>11</v>
+      </c>
+      <c r="L11">
+        <v>12</v>
+      </c>
+      <c r="M11">
+        <v>13</v>
+      </c>
+      <c r="N11">
+        <v>14</v>
+      </c>
+      <c r="O11">
+        <v>15</v>
+      </c>
+      <c r="P11">
+        <v>16</v>
+      </c>
+      <c r="Q11">
+        <v>17</v>
+      </c>
+      <c r="R11">
+        <v>1</v>
+      </c>
+      <c r="S11">
+        <v>2</v>
+      </c>
+      <c r="T11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:24">
+      <c r="A12" t="s">
+        <v>315</v>
+      </c>
+      <c r="C12" t="s">
+        <v>2</v>
+      </c>
+      <c r="E12" t="s">
+        <v>3</v>
+      </c>
+      <c r="G12" t="s">
+        <v>4</v>
+      </c>
+      <c r="I12" t="s">
+        <v>5</v>
+      </c>
+      <c r="K12" t="s">
         <v>304</v>
       </c>
-      <c r="K7" s="2"/>
-      <c r="L7" s="1" t="s">
+      <c r="L12" s="2"/>
+      <c r="M12" s="1" t="s">
         <v>309</v>
       </c>
-      <c r="M7" s="1" t="s">
+      <c r="N12" s="1" t="s">
         <v>310</v>
       </c>
-      <c r="N7" s="1" t="s">
+      <c r="O12" s="1" t="s">
         <v>311</v>
       </c>
-      <c r="O7" s="1" t="s">
+      <c r="P12" s="1" t="s">
         <v>312</v>
       </c>
-      <c r="P7" s="1" t="s">
+      <c r="Q12" s="3" t="s">
         <v>313</v>
       </c>
-      <c r="Q7" s="1" t="s">
-        <v>314</v>
-      </c>
-      <c r="R7" s="1" t="s">
-        <v>315</v>
-      </c>
-      <c r="S7" s="1" t="s">
-        <v>316</v>
-      </c>
-      <c r="T7" s="1" t="s">
+      <c r="R12" s="5" t="s">
         <v>317</v>
       </c>
-      <c r="U7" s="1" t="s">
+      <c r="S12" s="5" t="s">
         <v>318</v>
       </c>
-    </row>
-    <row r="8" spans="1:21">
-      <c r="A8" t="s">
+      <c r="T12" s="5" t="s">
+        <v>319</v>
+      </c>
+      <c r="U12" s="5" t="s">
+        <v>320</v>
+      </c>
+      <c r="V12" s="5" t="s">
+        <v>321</v>
+      </c>
+      <c r="W12" s="5" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="13" spans="1:24">
+      <c r="B13" t="s">
         <v>78</v>
       </c>
-      <c r="K8" s="2"/>
-    </row>
-    <row r="9" spans="1:21">
-      <c r="B9" t="s">
+      <c r="L13" s="2"/>
+      <c r="Q13" s="2"/>
+    </row>
+    <row r="14" spans="1:24">
+      <c r="C14" t="s">
         <v>305</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D14" t="s">
         <v>306</v>
       </c>
-      <c r="D9" t="s">
+      <c r="E14" t="s">
         <v>305</v>
       </c>
-      <c r="E9" t="s">
+      <c r="F14" t="s">
         <v>306</v>
       </c>
-      <c r="F9" t="s">
+      <c r="G14" t="s">
         <v>305</v>
       </c>
-      <c r="G9" t="s">
+      <c r="H14" t="s">
         <v>306</v>
       </c>
-      <c r="H9" t="s">
+      <c r="I14" t="s">
         <v>305</v>
       </c>
-      <c r="I9" t="s">
+      <c r="J14" t="s">
         <v>306</v>
       </c>
-      <c r="J9" t="s">
+      <c r="K14" t="s">
         <v>305</v>
       </c>
-      <c r="K9" s="2" t="s">
+      <c r="L14" s="2" t="s">
         <v>306</v>
       </c>
-    </row>
-    <row r="10" spans="1:21">
-      <c r="A10" t="s">
+      <c r="Q14" s="2"/>
+    </row>
+    <row r="15" spans="1:24" s="8" customFormat="1">
+      <c r="A15" s="8">
+        <v>1</v>
+      </c>
+      <c r="B15" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="B10">
+      <c r="C15" s="8">
         <v>14</v>
       </c>
-      <c r="C10">
+      <c r="D15" s="8">
         <v>33</v>
       </c>
-      <c r="D10">
+      <c r="E15" s="8">
         <v>9</v>
       </c>
-      <c r="E10">
+      <c r="F15" s="8">
         <v>21</v>
       </c>
-      <c r="F10">
+      <c r="G15" s="8">
         <v>2</v>
       </c>
-      <c r="G10">
+      <c r="H15" s="8">
         <v>5</v>
       </c>
-      <c r="H10">
+      <c r="I15" s="8">
         <v>4</v>
       </c>
-      <c r="I10">
+      <c r="J15" s="8">
         <v>9</v>
       </c>
-      <c r="J10">
+      <c r="K15" s="8">
         <v>14</v>
       </c>
-      <c r="K10" s="2">
+      <c r="L15" s="9">
         <v>33</v>
       </c>
-      <c r="L10">
-        <f>STANDARDIZE(B10,B$4,B$5)</f>
-        <v>-0.52954765511877711</v>
-      </c>
-      <c r="M10">
-        <f t="shared" ref="M10:U25" si="2">STANDARDIZE(C10,C$4,C$5)</f>
+      <c r="M15" s="8">
+        <f>STANDARDIZE(D15,D$9,D$10)</f>
         <v>-7.8997304592119968E-2</v>
       </c>
-      <c r="N10">
+      <c r="N15" s="8">
+        <f>STANDARDIZE(F15,F$9,F$10)</f>
+        <v>0.3503753231992241</v>
+      </c>
+      <c r="O15" s="8">
+        <f>STANDARDIZE(H15,H$9,H$10)</f>
+        <v>-0.48306751694697775</v>
+      </c>
+      <c r="P15" s="8">
+        <f>STANDARDIZE(J15,J$9,J$10)</f>
+        <v>1.7610282188688935</v>
+      </c>
+      <c r="Q15" s="9">
+        <f>STANDARDIZE(L15,L$9,L$10)</f>
+        <v>-0.23746913714629164</v>
+      </c>
+      <c r="R15" s="8">
+        <f>SUMXMY2($F$3:$J$3,M15:Q15)</f>
+        <v>4.402227672836112</v>
+      </c>
+      <c r="S15" s="8">
+        <f>SUMXMY2($F$4:$J$4,M15:Q15)</f>
+        <v>16.205716829074397</v>
+      </c>
+      <c r="T15" s="8">
+        <f>SUMXMY2($F$5:$J$5,M15:Q15)</f>
+        <v>3.5551086504993425</v>
+      </c>
+      <c r="U15" s="8">
+        <f>MIN(R15:T15)</f>
+        <v>3.5551086504993425</v>
+      </c>
+      <c r="V15" s="8">
+        <f>MATCH(U15,R15:T15, FALSE())</f>
+        <v>3</v>
+      </c>
+      <c r="X15" s="8" t="str">
+        <f>VLOOKUP(V15,$C$3:$E$5,3,FALSE())</f>
+        <v>Biological Chemistry</v>
+      </c>
+    </row>
+    <row r="16" spans="1:24" s="8" customFormat="1">
+      <c r="A16" s="8">
+        <v>2</v>
+      </c>
+      <c r="B16" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C16" s="8">
+        <v>61</v>
+      </c>
+      <c r="D16" s="8">
+        <v>37</v>
+      </c>
+      <c r="E16" s="8">
+        <v>26</v>
+      </c>
+      <c r="F16" s="8">
+        <v>16</v>
+      </c>
+      <c r="G16" s="8">
+        <v>14</v>
+      </c>
+      <c r="H16" s="8">
+        <v>8</v>
+      </c>
+      <c r="I16" s="8">
+        <v>13</v>
+      </c>
+      <c r="J16" s="8">
+        <v>8</v>
+      </c>
+      <c r="K16" s="8">
+        <v>52</v>
+      </c>
+      <c r="L16" s="9">
+        <v>31</v>
+      </c>
+      <c r="M16" s="8">
+        <f>STANDARDIZE(D16,D$9,D$10)</f>
+        <v>0.28965678350444118</v>
+      </c>
+      <c r="N16" s="8">
+        <f>STANDARDIZE(F16,F$9,F$10)</f>
+        <v>-4.5209719122480667E-2</v>
+      </c>
+      <c r="O16" s="8">
+        <f>STANDARDIZE(H16,H$9,H$10)</f>
+        <v>-2.1957614406680731E-2</v>
+      </c>
+      <c r="P16" s="8">
+        <f>STANDARDIZE(J16,J$9,J$10)</f>
+        <v>1.4186060651999419</v>
+      </c>
+      <c r="Q16" s="9">
+        <f>STANDARDIZE(L16,L$9,L$10)</f>
+        <v>-0.3458789606261205</v>
+      </c>
+      <c r="R16" s="8">
+        <f t="shared" ref="R16:R35" si="2">SUMXMY2($F$3:$J$3,M16:Q16)</f>
+        <v>5.0033879836858262</v>
+      </c>
+      <c r="S16" s="8">
+        <f t="shared" ref="S16:S35" si="3">SUMXMY2($F$4:$J$4,M16:Q16)</f>
+        <v>14.523090676776949</v>
+      </c>
+      <c r="T16" s="8">
+        <f t="shared" ref="T16:T35" si="4">SUMXMY2($F$5:$J$5,M16:Q16)</f>
+        <v>1.4006812665124366</v>
+      </c>
+      <c r="U16" s="8">
+        <f t="shared" ref="U16:U35" si="5">MIN(R16:T16)</f>
+        <v>1.4006812665124366</v>
+      </c>
+      <c r="V16" s="8">
+        <f t="shared" ref="V16:V35" si="6">MATCH(U16,R16:T16, FALSE())</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:22" s="8" customFormat="1">
+      <c r="A17" s="8">
+        <v>3</v>
+      </c>
+      <c r="B17" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C17" s="8">
+        <v>59</v>
+      </c>
+      <c r="D17" s="8">
+        <v>40</v>
+      </c>
+      <c r="E17" s="8">
+        <v>19</v>
+      </c>
+      <c r="F17" s="8">
+        <v>13</v>
+      </c>
+      <c r="G17" s="8">
+        <v>17</v>
+      </c>
+      <c r="H17" s="8">
+        <v>11</v>
+      </c>
+      <c r="I17" s="8">
+        <v>8</v>
+      </c>
+      <c r="J17" s="8">
+        <v>5</v>
+      </c>
+      <c r="K17" s="8">
+        <v>46</v>
+      </c>
+      <c r="L17" s="9">
+        <v>31</v>
+      </c>
+      <c r="M17" s="8">
+        <f>STANDARDIZE(D17,D$9,D$10)</f>
+        <v>0.56614734957686197</v>
+      </c>
+      <c r="N17" s="8">
+        <f>STANDARDIZE(F17,F$9,F$10)</f>
+        <v>-0.2825607445155035</v>
+      </c>
+      <c r="O17" s="8">
+        <f>STANDARDIZE(H17,H$9,H$10)</f>
+        <v>0.43915228813361629</v>
+      </c>
+      <c r="P17" s="8">
+        <f>STANDARDIZE(J17,J$9,J$10)</f>
+        <v>0.39133960419308744</v>
+      </c>
+      <c r="Q17" s="9">
+        <f>STANDARDIZE(L17,L$9,L$10)</f>
+        <v>-0.3458789606261205</v>
+      </c>
+      <c r="R17" s="8">
         <f t="shared" si="2"/>
-        <v>-0.29444413508864942</v>
-      </c>
-      <c r="O10">
+        <v>5.2273277495191302</v>
+      </c>
+      <c r="S17" s="8">
+        <f t="shared" si="3"/>
+        <v>10.952926019944336</v>
+      </c>
+      <c r="T17" s="8">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="U17" s="8">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="V17" s="8">
+        <f t="shared" si="6"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:22" s="6" customFormat="1">
+      <c r="A18" s="6">
+        <v>4</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C18" s="6">
+        <v>30</v>
+      </c>
+      <c r="D18" s="6">
+        <v>29</v>
+      </c>
+      <c r="E18" s="6">
+        <v>29</v>
+      </c>
+      <c r="F18" s="6">
+        <v>28</v>
+      </c>
+      <c r="G18" s="6">
+        <v>11</v>
+      </c>
+      <c r="H18" s="6">
+        <v>10</v>
+      </c>
+      <c r="I18" s="6">
+        <v>8</v>
+      </c>
+      <c r="J18" s="6">
+        <v>8</v>
+      </c>
+      <c r="K18" s="6">
+        <v>27</v>
+      </c>
+      <c r="L18" s="7">
+        <v>26</v>
+      </c>
+      <c r="M18" s="6">
+        <f>STANDARDIZE(D18,D$9,D$10)</f>
+        <v>-0.44765139268868109</v>
+      </c>
+      <c r="N18" s="6">
+        <f>STANDARDIZE(F18,F$9,F$10)</f>
+        <v>0.90419438244961081</v>
+      </c>
+      <c r="O18" s="6">
+        <f>STANDARDIZE(H18,H$9,H$10)</f>
+        <v>0.28544898728685059</v>
+      </c>
+      <c r="P18" s="6">
+        <f>STANDARDIZE(J18,J$9,J$10)</f>
+        <v>1.4186060651999419</v>
+      </c>
+      <c r="Q18" s="7">
+        <f>STANDARDIZE(L18,L$9,L$10)</f>
+        <v>-0.61690351932569254</v>
+      </c>
+      <c r="R18" s="6">
         <f t="shared" si="2"/>
+        <v>3.0417459352362948</v>
+      </c>
+      <c r="S18" s="6">
+        <f t="shared" si="3"/>
+        <v>19.106553724825186</v>
+      </c>
+      <c r="T18" s="6">
+        <f t="shared" si="4"/>
+        <v>3.5885310192162176</v>
+      </c>
+      <c r="U18" s="6">
+        <f t="shared" si="5"/>
+        <v>3.0417459352362948</v>
+      </c>
+      <c r="V18" s="6">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:22" s="8" customFormat="1">
+      <c r="A19" s="8">
+        <v>5</v>
+      </c>
+      <c r="B19" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C19" s="8">
+        <v>25</v>
+      </c>
+      <c r="D19" s="8">
+        <v>42</v>
+      </c>
+      <c r="E19" s="8">
+        <v>10</v>
+      </c>
+      <c r="F19" s="8">
+        <v>17</v>
+      </c>
+      <c r="G19" s="8">
+        <v>7</v>
+      </c>
+      <c r="H19" s="8">
+        <v>12</v>
+      </c>
+      <c r="I19" s="8">
+        <v>3</v>
+      </c>
+      <c r="J19" s="8">
+        <v>5</v>
+      </c>
+      <c r="K19" s="8">
+        <v>15</v>
+      </c>
+      <c r="L19" s="9">
+        <v>25</v>
+      </c>
+      <c r="M19" s="8">
+        <f>STANDARDIZE(D19,D$9,D$10)</f>
+        <v>0.75047439362514257</v>
+      </c>
+      <c r="N19" s="8">
+        <f>STANDARDIZE(F19,F$9,F$10)</f>
+        <v>3.390728934186029E-2</v>
+      </c>
+      <c r="O19" s="8">
+        <f>STANDARDIZE(H19,H$9,H$10)</f>
+        <v>0.59285558898038193</v>
+      </c>
+      <c r="P19" s="8">
+        <f>STANDARDIZE(J19,J$9,J$10)</f>
+        <v>0.39133960419308744</v>
+      </c>
+      <c r="Q19" s="9">
+        <f>STANDARDIZE(L19,L$9,L$10)</f>
+        <v>-0.67110843106560703</v>
+      </c>
+      <c r="R19" s="8">
+        <f t="shared" si="2"/>
+        <v>4.8834030672333224</v>
+      </c>
+      <c r="S19" s="8">
+        <f t="shared" si="3"/>
+        <v>13.970975821720804</v>
+      </c>
+      <c r="T19" s="8">
+        <f t="shared" si="4"/>
+        <v>0.26352738875466253</v>
+      </c>
+      <c r="U19" s="8">
+        <f t="shared" si="5"/>
+        <v>0.26352738875466253</v>
+      </c>
+      <c r="V19" s="8">
+        <f t="shared" si="6"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:22" s="8" customFormat="1">
+      <c r="A20" s="8">
+        <v>6</v>
+      </c>
+      <c r="B20" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="C20" s="8">
+        <v>23</v>
+      </c>
+      <c r="D20" s="8">
+        <v>47</v>
+      </c>
+      <c r="E20" s="8">
+        <v>9</v>
+      </c>
+      <c r="F20" s="8">
+        <v>18</v>
+      </c>
+      <c r="G20" s="8">
+        <v>1</v>
+      </c>
+      <c r="H20" s="8">
+        <v>2</v>
+      </c>
+      <c r="I20" s="8">
+        <v>1</v>
+      </c>
+      <c r="J20" s="8">
+        <v>2</v>
+      </c>
+      <c r="K20" s="8">
+        <v>15</v>
+      </c>
+      <c r="L20" s="9">
+        <v>31</v>
+      </c>
+      <c r="M20" s="8">
+        <f>STANDARDIZE(D20,D$9,D$10)</f>
+        <v>1.2112920037458441</v>
+      </c>
+      <c r="N20" s="8">
+        <f>STANDARDIZE(F20,F$9,F$10)</f>
+        <v>0.11302429780620124</v>
+      </c>
+      <c r="O20" s="8">
+        <f>STANDARDIZE(H20,H$9,H$10)</f>
+        <v>-0.94417741948727474</v>
+      </c>
+      <c r="P20" s="8">
+        <f>STANDARDIZE(J20,J$9,J$10)</f>
+        <v>-0.63592685681376715</v>
+      </c>
+      <c r="Q20" s="9">
+        <f>STANDARDIZE(L20,L$9,L$10)</f>
+        <v>-0.3458789606261205</v>
+      </c>
+      <c r="R20" s="8">
+        <f t="shared" si="2"/>
+        <v>4.9007598275257838</v>
+      </c>
+      <c r="S20" s="8">
+        <f t="shared" si="3"/>
+        <v>9.2715413443171357</v>
+      </c>
+      <c r="T20" s="8">
+        <f t="shared" si="4"/>
+        <v>3.5415766124075274</v>
+      </c>
+      <c r="U20" s="8">
+        <f t="shared" si="5"/>
+        <v>3.5415766124075274</v>
+      </c>
+      <c r="V20" s="8">
+        <f t="shared" si="6"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:22" s="10" customFormat="1">
+      <c r="A21" s="10">
+        <v>7</v>
+      </c>
+      <c r="B21" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="C21" s="10">
+        <v>0</v>
+      </c>
+      <c r="D21" s="10">
+        <v>0</v>
+      </c>
+      <c r="E21" s="10">
+        <v>0</v>
+      </c>
+      <c r="F21" s="10">
+        <v>0</v>
+      </c>
+      <c r="G21" s="10">
+        <v>0</v>
+      </c>
+      <c r="H21" s="10">
+        <v>0</v>
+      </c>
+      <c r="I21" s="10">
+        <v>0</v>
+      </c>
+      <c r="J21" s="10">
+        <v>0</v>
+      </c>
+      <c r="K21" s="10">
+        <v>1</v>
+      </c>
+      <c r="L21" s="11">
+        <v>100</v>
+      </c>
+      <c r="M21" s="10">
+        <f>STANDARDIZE(D21,D$9,D$10)</f>
+        <v>-3.1203935313887494</v>
+      </c>
+      <c r="N21" s="10">
+        <f>STANDARDIZE(F21,F$9,F$10)</f>
+        <v>-1.311081854551936</v>
+      </c>
+      <c r="O21" s="10">
+        <f>STANDARDIZE(H21,H$9,H$10)</f>
+        <v>-1.251584021180806</v>
+      </c>
+      <c r="P21" s="10">
+        <f>STANDARDIZE(J21,J$9,J$10)</f>
+        <v>-1.3207711641516702</v>
+      </c>
+      <c r="Q21" s="11">
+        <f>STANDARDIZE(L21,L$9,L$10)</f>
+        <v>3.3942599494279744</v>
+      </c>
+      <c r="R21" s="10">
+        <f t="shared" si="2"/>
+        <v>33.656066621724889</v>
+      </c>
+      <c r="S21" s="10">
+        <f t="shared" si="3"/>
+        <v>10.246737954441258</v>
+      </c>
+      <c r="T21" s="10">
+        <f t="shared" si="4"/>
+        <v>34.426990958038147</v>
+      </c>
+      <c r="U21" s="10">
+        <f t="shared" si="5"/>
+        <v>10.246737954441258</v>
+      </c>
+      <c r="V21" s="10">
+        <f t="shared" si="6"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:22" s="8" customFormat="1">
+      <c r="A22" s="8">
+        <v>8</v>
+      </c>
+      <c r="B22" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="C22" s="8">
+        <v>36</v>
+      </c>
+      <c r="D22" s="8">
+        <v>38</v>
+      </c>
+      <c r="E22" s="8">
+        <v>20</v>
+      </c>
+      <c r="F22" s="8">
+        <v>21</v>
+      </c>
+      <c r="G22" s="8">
+        <v>5</v>
+      </c>
+      <c r="H22" s="8">
+        <v>5</v>
+      </c>
+      <c r="I22" s="8">
+        <v>6</v>
+      </c>
+      <c r="J22" s="8">
+        <v>6</v>
+      </c>
+      <c r="K22" s="8">
+        <v>28</v>
+      </c>
+      <c r="L22" s="9">
+        <v>29</v>
+      </c>
+      <c r="M22" s="8">
+        <f>STANDARDIZE(D22,D$9,D$10)</f>
+        <v>0.38182030552858148</v>
+      </c>
+      <c r="N22" s="8">
+        <f>STANDARDIZE(F22,F$9,F$10)</f>
         <v>0.3503753231992241</v>
       </c>
-      <c r="P10">
+      <c r="O22" s="8">
+        <f>STANDARDIZE(H22,H$9,H$10)</f>
+        <v>-0.48306751694697775</v>
+      </c>
+      <c r="P22" s="8">
+        <f>STANDARDIZE(J22,J$9,J$10)</f>
+        <v>0.73376175786203901</v>
+      </c>
+      <c r="Q22" s="9">
+        <f>STANDARDIZE(L22,L$9,L$10)</f>
+        <v>-0.45428878410594931</v>
+      </c>
+      <c r="R22" s="8">
         <f t="shared" si="2"/>
-        <v>-0.6697421819723568</v>
-      </c>
-      <c r="Q10">
+        <v>2.2895655303320721</v>
+      </c>
+      <c r="S22" s="8">
+        <f t="shared" si="3"/>
+        <v>12.351151428192427</v>
+      </c>
+      <c r="T22" s="8">
+        <f t="shared" si="4"/>
+        <v>1.4140795150148584</v>
+      </c>
+      <c r="U22" s="8">
+        <f t="shared" si="5"/>
+        <v>1.4140795150148584</v>
+      </c>
+      <c r="V22" s="8">
+        <f t="shared" si="6"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:22" s="10" customFormat="1">
+      <c r="A23" s="10">
+        <v>9</v>
+      </c>
+      <c r="B23" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="C23" s="10">
+        <v>4</v>
+      </c>
+      <c r="D23" s="10">
+        <v>40</v>
+      </c>
+      <c r="E23" s="10">
+        <v>1</v>
+      </c>
+      <c r="F23" s="10">
+        <v>10</v>
+      </c>
+      <c r="G23" s="10">
+        <v>0</v>
+      </c>
+      <c r="H23" s="10">
+        <v>0</v>
+      </c>
+      <c r="I23" s="10">
+        <v>0</v>
+      </c>
+      <c r="J23" s="10">
+        <v>0</v>
+      </c>
+      <c r="K23" s="10">
+        <v>5</v>
+      </c>
+      <c r="L23" s="11">
+        <v>50</v>
+      </c>
+      <c r="M23" s="10">
+        <f>STANDARDIZE(D23,D$9,D$10)</f>
+        <v>0.56614734957686197</v>
+      </c>
+      <c r="N23" s="10">
+        <f>STANDARDIZE(F23,F$9,F$10)</f>
+        <v>-0.51991176990852639</v>
+      </c>
+      <c r="O23" s="10">
+        <f>STANDARDIZE(H23,H$9,H$10)</f>
+        <v>-1.251584021180806</v>
+      </c>
+      <c r="P23" s="10">
+        <f>STANDARDIZE(J23,J$9,J$10)</f>
+        <v>-1.3207711641516702</v>
+      </c>
+      <c r="Q23" s="11">
+        <f>STANDARDIZE(L23,L$9,L$10)</f>
+        <v>0.68401436243225344</v>
+      </c>
+      <c r="R23" s="10">
         <f t="shared" si="2"/>
-        <v>-0.48306751694697775</v>
-      </c>
-      <c r="R10">
+        <v>8.7080291332152164</v>
+      </c>
+      <c r="S23" s="10">
+        <f t="shared" si="3"/>
+        <v>2.7002046873997614</v>
+      </c>
+      <c r="T23" s="10">
+        <f t="shared" si="4"/>
+        <v>6.9069283168515696</v>
+      </c>
+      <c r="U23" s="10">
+        <f t="shared" si="5"/>
+        <v>2.7002046873997614</v>
+      </c>
+      <c r="V23" s="10">
+        <f t="shared" si="6"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:22" s="6" customFormat="1">
+      <c r="A24" s="6">
+        <v>10</v>
+      </c>
+      <c r="B24" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="C24" s="6">
+        <v>13</v>
+      </c>
+      <c r="D24" s="6">
+        <v>24</v>
+      </c>
+      <c r="E24" s="6">
+        <v>24</v>
+      </c>
+      <c r="F24" s="6">
+        <v>44</v>
+      </c>
+      <c r="G24" s="6">
+        <v>2</v>
+      </c>
+      <c r="H24" s="6">
+        <v>4</v>
+      </c>
+      <c r="I24" s="6">
+        <v>2</v>
+      </c>
+      <c r="J24" s="6">
+        <v>4</v>
+      </c>
+      <c r="K24" s="6">
+        <v>13</v>
+      </c>
+      <c r="L24" s="7">
+        <v>24</v>
+      </c>
+      <c r="M24" s="6">
+        <f>STANDARDIZE(D24,D$9,D$10)</f>
+        <v>-0.90846900280938248</v>
+      </c>
+      <c r="N24" s="6">
+        <f>STANDARDIZE(F24,F$9,F$10)</f>
+        <v>2.1700665178790661</v>
+      </c>
+      <c r="O24" s="6">
+        <f>STANDARDIZE(H24,H$9,H$10)</f>
+        <v>-0.63677081779374334</v>
+      </c>
+      <c r="P24" s="6">
+        <f>STANDARDIZE(J24,J$9,J$10)</f>
+        <v>4.8917450524135916E-2</v>
+      </c>
+      <c r="Q24" s="7">
+        <f>STANDARDIZE(L24,L$9,L$10)</f>
+        <v>-0.7253133428055214</v>
+      </c>
+      <c r="R24" s="6">
         <f t="shared" si="2"/>
-        <v>0.19462473604038072</v>
-      </c>
-      <c r="S10">
+        <v>0.82456040563119315</v>
+      </c>
+      <c r="S24" s="6">
+        <f t="shared" si="3"/>
+        <v>19.989594456846646</v>
+      </c>
+      <c r="T24" s="6">
+        <f t="shared" si="4"/>
+        <v>9.6087077865375168</v>
+      </c>
+      <c r="U24" s="6">
+        <f t="shared" si="5"/>
+        <v>0.82456040563119315</v>
+      </c>
+      <c r="V24" s="6">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:22" s="6" customFormat="1">
+      <c r="A25" s="6">
+        <v>11</v>
+      </c>
+      <c r="B25" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="C25" s="6">
+        <v>24</v>
+      </c>
+      <c r="D25" s="6">
+        <v>21</v>
+      </c>
+      <c r="E25" s="6">
+        <v>44</v>
+      </c>
+      <c r="F25" s="6">
+        <v>39</v>
+      </c>
+      <c r="G25" s="6">
+        <v>14</v>
+      </c>
+      <c r="H25" s="6">
+        <v>12</v>
+      </c>
+      <c r="I25" s="6">
+        <v>6</v>
+      </c>
+      <c r="J25" s="6">
+        <v>5</v>
+      </c>
+      <c r="K25" s="6">
+        <v>26</v>
+      </c>
+      <c r="L25" s="7">
+        <v>23</v>
+      </c>
+      <c r="M25" s="6">
+        <f>STANDARDIZE(D25,D$9,D$10)</f>
+        <v>-1.1849595688818033</v>
+      </c>
+      <c r="N25" s="6">
+        <f>STANDARDIZE(F25,F$9,F$10)</f>
+        <v>1.7744814755573612</v>
+      </c>
+      <c r="O25" s="6">
+        <f>STANDARDIZE(H25,H$9,H$10)</f>
+        <v>0.59285558898038193</v>
+      </c>
+      <c r="P25" s="6">
+        <f>STANDARDIZE(J25,J$9,J$10)</f>
+        <v>0.39133960419308744</v>
+      </c>
+      <c r="Q25" s="7">
+        <f>STANDARDIZE(L25,L$9,L$10)</f>
+        <v>-0.77951825454543577</v>
+      </c>
+      <c r="R25" s="6">
         <f t="shared" si="2"/>
-        <v>1.7610282188688935</v>
-      </c>
-      <c r="T10">
+        <v>2.4438528982670915</v>
+      </c>
+      <c r="S25" s="6">
+        <f t="shared" si="3"/>
+        <v>21.307917387879737</v>
+      </c>
+      <c r="T25" s="6">
+        <f t="shared" si="4"/>
+        <v>7.5094658769581359</v>
+      </c>
+      <c r="U25" s="6">
+        <f t="shared" si="5"/>
+        <v>2.4438528982670915</v>
+      </c>
+      <c r="V25" s="6">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:22" s="10" customFormat="1">
+      <c r="A26" s="10">
+        <v>12</v>
+      </c>
+      <c r="B26" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="C26" s="10">
+        <v>12</v>
+      </c>
+      <c r="D26" s="10">
+        <v>29</v>
+      </c>
+      <c r="E26" s="10">
+        <v>0</v>
+      </c>
+      <c r="F26" s="10">
+        <v>0</v>
+      </c>
+      <c r="G26" s="10">
+        <v>1</v>
+      </c>
+      <c r="H26" s="10">
+        <v>2</v>
+      </c>
+      <c r="I26" s="10">
+        <v>0</v>
+      </c>
+      <c r="J26" s="10">
+        <v>0</v>
+      </c>
+      <c r="K26" s="10">
+        <v>28</v>
+      </c>
+      <c r="L26" s="11">
+        <v>68</v>
+      </c>
+      <c r="M26" s="10">
+        <f>STANDARDIZE(D26,D$9,D$10)</f>
+        <v>-0.44765139268868109</v>
+      </c>
+      <c r="N26" s="10">
+        <f>STANDARDIZE(F26,F$9,F$10)</f>
+        <v>-1.311081854551936</v>
+      </c>
+      <c r="O26" s="10">
+        <f>STANDARDIZE(H26,H$9,H$10)</f>
+        <v>-0.94417741948727474</v>
+      </c>
+      <c r="P26" s="10">
+        <f>STANDARDIZE(J26,J$9,J$10)</f>
+        <v>-1.3207711641516702</v>
+      </c>
+      <c r="Q26" s="11">
+        <f>STANDARDIZE(L26,L$9,L$10)</f>
+        <v>1.6597027737507128</v>
+      </c>
+      <c r="R26" s="10">
         <f t="shared" si="2"/>
-        <v>-0.49283160921745228</v>
-      </c>
-      <c r="U10">
-        <f>STANDARDIZE(K10,K$4,K$5)</f>
+        <v>14.829864808128864</v>
+      </c>
+      <c r="S26" s="10">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="T26" s="10">
+        <f t="shared" si="4"/>
+        <v>10.952926019944336</v>
+      </c>
+      <c r="U26" s="10">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="V26" s="10">
+        <f t="shared" si="6"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:22" s="8" customFormat="1">
+      <c r="A27" s="8">
+        <v>13</v>
+      </c>
+      <c r="B27" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="C27" s="8">
+        <v>18</v>
+      </c>
+      <c r="D27" s="8">
+        <v>29</v>
+      </c>
+      <c r="E27" s="8">
+        <v>7</v>
+      </c>
+      <c r="F27" s="8">
+        <v>11</v>
+      </c>
+      <c r="G27" s="8">
+        <v>9</v>
+      </c>
+      <c r="H27" s="8">
+        <v>14</v>
+      </c>
+      <c r="I27" s="8">
+        <v>0</v>
+      </c>
+      <c r="J27" s="8">
+        <v>0</v>
+      </c>
+      <c r="K27" s="8">
+        <v>29</v>
+      </c>
+      <c r="L27" s="9">
+        <v>46</v>
+      </c>
+      <c r="M27" s="8">
+        <f>STANDARDIZE(D27,D$9,D$10)</f>
+        <v>-0.44765139268868109</v>
+      </c>
+      <c r="N27" s="8">
+        <f>STANDARDIZE(F27,F$9,F$10)</f>
+        <v>-0.44079476144418545</v>
+      </c>
+      <c r="O27" s="8">
+        <f>STANDARDIZE(H27,H$9,H$10)</f>
+        <v>0.90026219067391322</v>
+      </c>
+      <c r="P27" s="8">
+        <f>STANDARDIZE(J27,J$9,J$10)</f>
+        <v>-1.3207711641516702</v>
+      </c>
+      <c r="Q27" s="9">
+        <f>STANDARDIZE(L27,L$9,L$10)</f>
+        <v>0.46719471547259578</v>
+      </c>
+      <c r="R27" s="8">
+        <f t="shared" si="2"/>
+        <v>9.0277530601039633</v>
+      </c>
+      <c r="S27" s="8">
+        <f t="shared" si="3"/>
+        <v>5.5814325690197384</v>
+      </c>
+      <c r="T27" s="8">
+        <f t="shared" si="4"/>
+        <v>4.8578603220000618</v>
+      </c>
+      <c r="U27" s="8">
+        <f t="shared" si="5"/>
+        <v>4.8578603220000618</v>
+      </c>
+      <c r="V27" s="8">
+        <f t="shared" si="6"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:22" s="8" customFormat="1">
+      <c r="A28" s="8">
+        <v>14</v>
+      </c>
+      <c r="B28" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="C28" s="8">
+        <v>73</v>
+      </c>
+      <c r="D28" s="8">
+        <v>38</v>
+      </c>
+      <c r="E28" s="8">
+        <v>16</v>
+      </c>
+      <c r="F28" s="8">
+        <v>8</v>
+      </c>
+      <c r="G28" s="8">
+        <v>31</v>
+      </c>
+      <c r="H28" s="8">
+        <v>16</v>
+      </c>
+      <c r="I28" s="8">
+        <v>6</v>
+      </c>
+      <c r="J28" s="8">
+        <v>3</v>
+      </c>
+      <c r="K28" s="8">
+        <v>66</v>
+      </c>
+      <c r="L28" s="9">
+        <v>34</v>
+      </c>
+      <c r="M28" s="8">
+        <f>STANDARDIZE(D28,D$9,D$10)</f>
+        <v>0.38182030552858148</v>
+      </c>
+      <c r="N28" s="8">
+        <f>STANDARDIZE(F28,F$9,F$10)</f>
+        <v>-0.67814578683720828</v>
+      </c>
+      <c r="O28" s="8">
+        <f>STANDARDIZE(H28,H$9,H$10)</f>
+        <v>1.2076687923674445</v>
+      </c>
+      <c r="P28" s="8">
+        <f>STANDARDIZE(J28,J$9,J$10)</f>
+        <v>-0.29350470314481564</v>
+      </c>
+      <c r="Q28" s="9">
+        <f>STANDARDIZE(L28,L$9,L$10)</f>
+        <v>-0.18326422540637724</v>
+      </c>
+      <c r="R28" s="8">
+        <f t="shared" si="2"/>
+        <v>8.8140530404315776</v>
+      </c>
+      <c r="S28" s="8">
+        <f t="shared" si="3"/>
+        <v>10.170877225322755</v>
+      </c>
+      <c r="T28" s="8">
+        <f t="shared" si="4"/>
+        <v>1.2765368795597449</v>
+      </c>
+      <c r="U28" s="8">
+        <f t="shared" si="5"/>
+        <v>1.2765368795597449</v>
+      </c>
+      <c r="V28" s="8">
+        <f t="shared" si="6"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:22" s="10" customFormat="1">
+      <c r="A29" s="10">
+        <v>15</v>
+      </c>
+      <c r="B29" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="C29" s="10">
+        <v>5</v>
+      </c>
+      <c r="D29" s="10">
+        <v>45</v>
+      </c>
+      <c r="E29" s="10">
+        <v>0</v>
+      </c>
+      <c r="F29" s="10">
+        <v>0</v>
+      </c>
+      <c r="G29" s="10">
+        <v>0</v>
+      </c>
+      <c r="H29" s="10">
+        <v>0</v>
+      </c>
+      <c r="I29" s="10">
+        <v>0</v>
+      </c>
+      <c r="J29" s="10">
+        <v>0</v>
+      </c>
+      <c r="K29" s="10">
+        <v>6</v>
+      </c>
+      <c r="L29" s="11">
+        <v>55</v>
+      </c>
+      <c r="M29" s="10">
+        <f>STANDARDIZE(D29,D$9,D$10)</f>
+        <v>1.0269649596975634</v>
+      </c>
+      <c r="N29" s="10">
+        <f>STANDARDIZE(F29,F$9,F$10)</f>
+        <v>-1.311081854551936</v>
+      </c>
+      <c r="O29" s="10">
+        <f>STANDARDIZE(H29,H$9,H$10)</f>
+        <v>-1.251584021180806</v>
+      </c>
+      <c r="P29" s="10">
+        <f>STANDARDIZE(J29,J$9,J$10)</f>
+        <v>-1.3207711641516702</v>
+      </c>
+      <c r="Q29" s="11">
+        <f>STANDARDIZE(L29,L$9,L$10)</f>
+        <v>0.95503892113182554</v>
+      </c>
+      <c r="R29" s="10">
+        <f t="shared" si="2"/>
+        <v>14.304109800243904</v>
+      </c>
+      <c r="S29" s="10">
+        <f t="shared" si="3"/>
+        <v>2.7655433506773717</v>
+      </c>
+      <c r="T29" s="10">
+        <f t="shared" si="4"/>
+        <v>8.7525084293817415</v>
+      </c>
+      <c r="U29" s="10">
+        <f t="shared" si="5"/>
+        <v>2.7655433506773717</v>
+      </c>
+      <c r="V29" s="10">
+        <f t="shared" si="6"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:22" s="8" customFormat="1">
+      <c r="A30" s="8">
+        <v>16</v>
+      </c>
+      <c r="B30" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="C30" s="8">
+        <v>21</v>
+      </c>
+      <c r="D30" s="8">
+        <v>40</v>
+      </c>
+      <c r="E30" s="8">
+        <v>5</v>
+      </c>
+      <c r="F30" s="8">
+        <v>10</v>
+      </c>
+      <c r="G30" s="8">
+        <v>8</v>
+      </c>
+      <c r="H30" s="8">
+        <v>15</v>
+      </c>
+      <c r="I30" s="8">
+        <v>1</v>
+      </c>
+      <c r="J30" s="8">
+        <v>2</v>
+      </c>
+      <c r="K30" s="8">
+        <v>17</v>
+      </c>
+      <c r="L30" s="9">
+        <v>33</v>
+      </c>
+      <c r="M30" s="8">
+        <f>STANDARDIZE(D30,D$9,D$10)</f>
+        <v>0.56614734957686197</v>
+      </c>
+      <c r="N30" s="8">
+        <f>STANDARDIZE(F30,F$9,F$10)</f>
+        <v>-0.51991176990852639</v>
+      </c>
+      <c r="O30" s="8">
+        <f>STANDARDIZE(H30,H$9,H$10)</f>
+        <v>1.0539654915206789</v>
+      </c>
+      <c r="P30" s="8">
+        <f>STANDARDIZE(J30,J$9,J$10)</f>
+        <v>-0.63592685681376715</v>
+      </c>
+      <c r="Q30" s="9">
+        <f>STANDARDIZE(L30,L$9,L$10)</f>
         <v>-0.23746913714629164</v>
       </c>
-    </row>
-    <row r="11" spans="1:21">
-      <c r="A11" t="s">
+      <c r="R30" s="8">
+        <f t="shared" si="2"/>
+        <v>8.2331710652131935</v>
+      </c>
+      <c r="S30" s="8">
+        <f t="shared" si="3"/>
+        <v>9.7145860702549189</v>
+      </c>
+      <c r="T30" s="8">
+        <f t="shared" si="4"/>
+        <v>1.5013598560506556</v>
+      </c>
+      <c r="U30" s="8">
+        <f t="shared" si="5"/>
+        <v>1.5013598560506556</v>
+      </c>
+      <c r="V30" s="8">
+        <f t="shared" si="6"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:22" s="8" customFormat="1">
+      <c r="A31" s="8">
+        <v>17</v>
+      </c>
+      <c r="B31" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="C31" s="8">
+        <v>16</v>
+      </c>
+      <c r="D31" s="8">
+        <v>43</v>
+      </c>
+      <c r="E31" s="8">
+        <v>2</v>
+      </c>
+      <c r="F31" s="8">
+        <v>5</v>
+      </c>
+      <c r="G31" s="8">
+        <v>4</v>
+      </c>
+      <c r="H31" s="8">
         <v>11</v>
       </c>
-      <c r="B11">
-        <v>61</v>
-      </c>
-      <c r="C11">
-        <v>37</v>
-      </c>
-      <c r="D11">
-        <v>26</v>
-      </c>
-      <c r="E11">
+      <c r="I31" s="8">
+        <v>3</v>
+      </c>
+      <c r="J31" s="8">
+        <v>8</v>
+      </c>
+      <c r="K31" s="8">
+        <v>12</v>
+      </c>
+      <c r="L31" s="9">
+        <v>32</v>
+      </c>
+      <c r="M31" s="8">
+        <f t="shared" ref="M31:M35" si="7">STANDARDIZE(D31,D$9,D$10)</f>
+        <v>0.84263791564928292</v>
+      </c>
+      <c r="N31" s="8">
+        <f t="shared" ref="N31:N35" si="8">STANDARDIZE(F31,F$9,F$10)</f>
+        <v>-0.91549681223023116</v>
+      </c>
+      <c r="O31" s="8">
+        <f t="shared" ref="O31:O35" si="9">STANDARDIZE(H31,H$9,H$10)</f>
+        <v>0.43915228813361629</v>
+      </c>
+      <c r="P31" s="8">
+        <f t="shared" ref="P31:P35" si="10">STANDARDIZE(J31,J$9,J$10)</f>
+        <v>1.4186060651999419</v>
+      </c>
+      <c r="Q31" s="9">
+        <f t="shared" ref="Q31:Q35" si="11">STANDARDIZE(L31,L$9,L$10)</f>
+        <v>-0.29167404888620607</v>
+      </c>
+      <c r="R31" s="8">
+        <f t="shared" si="2"/>
+        <v>10.208487964825309</v>
+      </c>
+      <c r="S31" s="8">
+        <f t="shared" si="3"/>
+        <v>15.046994213521099</v>
+      </c>
+      <c r="T31" s="8">
+        <f t="shared" si="4"/>
+        <v>1.5352696533075092</v>
+      </c>
+      <c r="U31" s="8">
+        <f t="shared" si="5"/>
+        <v>1.5352696533075092</v>
+      </c>
+      <c r="V31" s="8">
+        <f t="shared" si="6"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:22" s="8" customFormat="1">
+      <c r="A32" s="8">
+        <v>18</v>
+      </c>
+      <c r="B32" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="C32" s="8">
         <v>16</v>
       </c>
-      <c r="F11">
-        <v>14</v>
-      </c>
-      <c r="G11">
-        <v>8</v>
-      </c>
-      <c r="H11">
-        <v>13</v>
-      </c>
-      <c r="I11">
-        <v>8</v>
-      </c>
-      <c r="J11">
-        <v>52</v>
-      </c>
-      <c r="K11" s="2">
-        <v>31</v>
-      </c>
-      <c r="L11">
-        <f t="shared" ref="L11:L30" si="3">STANDARDIZE(B11,B$4,B$5)</f>
-        <v>1.9014455337288181</v>
-      </c>
-      <c r="M11">
-        <f t="shared" si="2"/>
-        <v>0.28965678350444118</v>
-      </c>
-      <c r="N11">
-        <f t="shared" si="2"/>
-        <v>1.18607074134301</v>
-      </c>
-      <c r="O11">
-        <f t="shared" si="2"/>
-        <v>-4.5209719122480667E-2</v>
-      </c>
-      <c r="P11">
-        <f t="shared" si="2"/>
-        <v>0.87865258735822949</v>
-      </c>
-      <c r="Q11">
-        <f t="shared" si="2"/>
-        <v>-2.1957614406680731E-2</v>
-      </c>
-      <c r="R11">
-        <f t="shared" si="2"/>
-        <v>2.8220586725855208</v>
-      </c>
-      <c r="S11">
-        <f t="shared" si="2"/>
-        <v>1.4186060651999419</v>
-      </c>
-      <c r="T11">
-        <f t="shared" si="2"/>
-        <v>1.8342667585667307</v>
-      </c>
-      <c r="U11">
-        <f t="shared" si="2"/>
-        <v>-0.3458789606261205</v>
-      </c>
-    </row>
-    <row r="12" spans="1:21">
-      <c r="A12" t="s">
-        <v>16</v>
-      </c>
-      <c r="B12">
-        <v>59</v>
-      </c>
-      <c r="C12">
-        <v>40</v>
-      </c>
-      <c r="D12">
-        <v>19</v>
-      </c>
-      <c r="E12">
-        <v>13</v>
-      </c>
-      <c r="F12">
+      <c r="D32" s="8">
+        <v>27</v>
+      </c>
+      <c r="E32" s="8">
+        <v>10</v>
+      </c>
+      <c r="F32" s="8">
         <v>17</v>
       </c>
-      <c r="G12">
-        <v>11</v>
-      </c>
-      <c r="H12">
-        <v>8</v>
-      </c>
-      <c r="I12">
+      <c r="G32" s="8">
+        <v>15</v>
+      </c>
+      <c r="H32" s="8">
+        <v>25</v>
+      </c>
+      <c r="I32" s="8">
+        <v>3</v>
+      </c>
+      <c r="J32" s="8">
         <v>5</v>
       </c>
-      <c r="J12">
-        <v>46</v>
-      </c>
-      <c r="K12" s="2">
-        <v>31</v>
-      </c>
-      <c r="L12">
-        <f t="shared" si="3"/>
-        <v>1.7979990150544525</v>
-      </c>
-      <c r="M12">
-        <f t="shared" si="2"/>
-        <v>0.56614734957686197</v>
-      </c>
-      <c r="N12">
-        <f t="shared" si="2"/>
-        <v>0.57644696869467971</v>
-      </c>
-      <c r="O12">
-        <f t="shared" si="2"/>
-        <v>-0.2825607445155035</v>
-      </c>
-      <c r="P12">
-        <f t="shared" si="2"/>
-        <v>1.2657512796908763</v>
-      </c>
-      <c r="Q12">
-        <f t="shared" si="2"/>
-        <v>0.43915228813361629</v>
-      </c>
-      <c r="R12">
-        <f t="shared" si="2"/>
-        <v>1.3623731522826652</v>
-      </c>
-      <c r="S12">
-        <f t="shared" si="2"/>
-        <v>0.39133960419308744</v>
-      </c>
-      <c r="T12">
-        <f t="shared" si="2"/>
-        <v>1.4668301741797545</v>
-      </c>
-      <c r="U12">
-        <f t="shared" si="2"/>
-        <v>-0.3458789606261205</v>
-      </c>
-    </row>
-    <row r="13" spans="1:21">
-      <c r="A13" t="s">
-        <v>20</v>
-      </c>
-      <c r="B13">
-        <v>30</v>
-      </c>
-      <c r="C13">
-        <v>29</v>
-      </c>
-      <c r="D13">
-        <v>29</v>
-      </c>
-      <c r="E13">
-        <v>28</v>
-      </c>
-      <c r="F13">
-        <v>11</v>
-      </c>
-      <c r="G13">
-        <v>10</v>
-      </c>
-      <c r="H13">
-        <v>8</v>
-      </c>
-      <c r="I13">
-        <v>8</v>
-      </c>
-      <c r="J13">
-        <v>27</v>
-      </c>
-      <c r="K13" s="2">
-        <v>26</v>
-      </c>
-      <c r="L13">
-        <f t="shared" si="3"/>
-        <v>0.29802449427614902</v>
-      </c>
-      <c r="M13">
-        <f t="shared" si="2"/>
-        <v>-0.44765139268868109</v>
-      </c>
-      <c r="N13">
-        <f t="shared" si="2"/>
-        <v>1.4473380724780089</v>
-      </c>
-      <c r="O13">
-        <f t="shared" si="2"/>
-        <v>0.90419438244961081</v>
-      </c>
-      <c r="P13">
-        <f t="shared" si="2"/>
-        <v>0.49155389502558294</v>
-      </c>
-      <c r="Q13">
-        <f t="shared" si="2"/>
-        <v>0.28544898728685059</v>
-      </c>
-      <c r="R13">
-        <f t="shared" si="2"/>
-        <v>1.3623731522826652</v>
-      </c>
-      <c r="S13">
-        <f t="shared" si="2"/>
-        <v>1.4186060651999419</v>
-      </c>
-      <c r="T13">
-        <f t="shared" si="2"/>
-        <v>0.30328099028766298</v>
-      </c>
-      <c r="U13">
-        <f t="shared" si="2"/>
-        <v>-0.61690351932569254</v>
-      </c>
-    </row>
-    <row r="14" spans="1:21">
-      <c r="A14" t="s">
-        <v>24</v>
-      </c>
-      <c r="B14">
+      <c r="K32" s="8">
+        <v>15</v>
+      </c>
+      <c r="L32" s="9">
         <v>25</v>
       </c>
-      <c r="C14">
-        <v>42</v>
-      </c>
-      <c r="D14">
-        <v>10</v>
-      </c>
-      <c r="E14">
-        <v>17</v>
-      </c>
-      <c r="F14">
-        <v>7</v>
-      </c>
-      <c r="G14">
-        <v>12</v>
-      </c>
-      <c r="H14">
-        <v>3</v>
-      </c>
-      <c r="I14">
-        <v>5</v>
-      </c>
-      <c r="J14">
-        <v>15</v>
-      </c>
-      <c r="K14" s="2">
-        <v>25</v>
-      </c>
-      <c r="L14">
-        <f t="shared" si="3"/>
-        <v>3.9408197590234617E-2</v>
-      </c>
-      <c r="M14">
-        <f t="shared" si="2"/>
-        <v>0.75047439362514257</v>
-      </c>
-      <c r="N14">
-        <f t="shared" si="2"/>
-        <v>-0.2073550247103165</v>
-      </c>
-      <c r="O14">
-        <f t="shared" si="2"/>
+      <c r="M32" s="8">
+        <f t="shared" si="7"/>
+        <v>-0.63197843673696164</v>
+      </c>
+      <c r="N32" s="8">
+        <f t="shared" si="8"/>
         <v>3.390728934186029E-2</v>
       </c>
-      <c r="P14">
-        <f t="shared" si="2"/>
-        <v>-2.4577694751279175E-2</v>
-      </c>
-      <c r="Q14">
-        <f t="shared" si="2"/>
-        <v>0.59285558898038193</v>
-      </c>
-      <c r="R14">
-        <f t="shared" si="2"/>
-        <v>-9.7312368020190429E-2</v>
-      </c>
-      <c r="S14">
-        <f t="shared" si="2"/>
-        <v>0.39133960419308744</v>
-      </c>
-      <c r="T14">
-        <f t="shared" si="2"/>
-        <v>-0.43159217848628961</v>
-      </c>
-      <c r="U14">
-        <f t="shared" si="2"/>
-        <v>-0.67110843106560703</v>
-      </c>
-    </row>
-    <row r="15" spans="1:21">
-      <c r="A15" t="s">
-        <v>28</v>
-      </c>
-      <c r="B15">
-        <v>23</v>
-      </c>
-      <c r="C15">
-        <v>47</v>
-      </c>
-      <c r="D15">
-        <v>9</v>
-      </c>
-      <c r="E15">
-        <v>18</v>
-      </c>
-      <c r="F15">
-        <v>1</v>
-      </c>
-      <c r="G15">
-        <v>2</v>
-      </c>
-      <c r="H15">
-        <v>1</v>
-      </c>
-      <c r="I15">
-        <v>2</v>
-      </c>
-      <c r="J15">
-        <v>15</v>
-      </c>
-      <c r="K15" s="2">
-        <v>31</v>
-      </c>
-      <c r="L15">
-        <f t="shared" si="3"/>
-        <v>-6.4038321084131142E-2</v>
-      </c>
-      <c r="M15">
-        <f t="shared" si="2"/>
-        <v>1.2112920037458441</v>
-      </c>
-      <c r="N15">
-        <f t="shared" si="2"/>
-        <v>-0.29444413508864942</v>
-      </c>
-      <c r="O15">
-        <f t="shared" si="2"/>
-        <v>0.11302429780620124</v>
-      </c>
-      <c r="P15">
-        <f t="shared" si="2"/>
-        <v>-0.79877507941657233</v>
-      </c>
-      <c r="Q15">
-        <f t="shared" si="2"/>
-        <v>-0.94417741948727474</v>
-      </c>
-      <c r="R15">
-        <f t="shared" si="2"/>
-        <v>-0.68118657614133271</v>
-      </c>
-      <c r="S15">
-        <f t="shared" si="2"/>
-        <v>-0.63592685681376715</v>
-      </c>
-      <c r="T15">
-        <f t="shared" si="2"/>
-        <v>-0.43159217848628961</v>
-      </c>
-      <c r="U15">
-        <f t="shared" si="2"/>
-        <v>-0.3458789606261205</v>
-      </c>
-    </row>
-    <row r="16" spans="1:21">
-      <c r="A16" t="s">
-        <v>33</v>
-      </c>
-      <c r="B16">
-        <v>0</v>
-      </c>
-      <c r="C16">
-        <v>0</v>
-      </c>
-      <c r="D16">
-        <v>0</v>
-      </c>
-      <c r="E16">
-        <v>0</v>
-      </c>
-      <c r="F16">
-        <v>0</v>
-      </c>
-      <c r="G16">
-        <v>0</v>
-      </c>
-      <c r="H16">
-        <v>0</v>
-      </c>
-      <c r="I16">
-        <v>0</v>
-      </c>
-      <c r="J16">
-        <v>1</v>
-      </c>
-      <c r="K16" s="2">
-        <v>100</v>
-      </c>
-      <c r="L16">
-        <f t="shared" si="3"/>
-        <v>-1.2536732858393373</v>
-      </c>
-      <c r="M16">
-        <f t="shared" si="2"/>
-        <v>-3.1203935313887494</v>
-      </c>
-      <c r="N16">
-        <f t="shared" si="2"/>
-        <v>-1.0782461284936455</v>
-      </c>
-      <c r="O16">
-        <f t="shared" si="2"/>
-        <v>-1.311081854551936</v>
-      </c>
-      <c r="P16">
-        <f t="shared" si="2"/>
-        <v>-0.92780797686078786</v>
-      </c>
-      <c r="Q16">
-        <f t="shared" si="2"/>
-        <v>-1.251584021180806</v>
-      </c>
-      <c r="R16">
-        <f t="shared" si="2"/>
-        <v>-0.97312368020190387</v>
-      </c>
-      <c r="S16">
-        <f t="shared" si="2"/>
-        <v>-1.3207711641516702</v>
-      </c>
-      <c r="T16">
-        <f t="shared" si="2"/>
-        <v>-1.2889442087225675</v>
-      </c>
-      <c r="U16">
-        <f t="shared" si="2"/>
-        <v>3.3942599494279744</v>
-      </c>
-    </row>
-    <row r="17" spans="1:21">
-      <c r="A17" t="s">
-        <v>36</v>
-      </c>
-      <c r="B17">
-        <v>36</v>
-      </c>
-      <c r="C17">
-        <v>38</v>
-      </c>
-      <c r="D17">
-        <v>20</v>
-      </c>
-      <c r="E17">
-        <v>21</v>
-      </c>
-      <c r="F17">
-        <v>5</v>
-      </c>
-      <c r="G17">
-        <v>5</v>
-      </c>
-      <c r="H17">
-        <v>6</v>
-      </c>
-      <c r="I17">
-        <v>6</v>
-      </c>
-      <c r="J17">
-        <v>28</v>
-      </c>
-      <c r="K17" s="2">
-        <v>29</v>
-      </c>
-      <c r="L17">
-        <f t="shared" si="3"/>
-        <v>0.60836405029924634</v>
-      </c>
-      <c r="M17">
-        <f t="shared" si="2"/>
-        <v>0.38182030552858148</v>
-      </c>
-      <c r="N17">
-        <f t="shared" si="2"/>
-        <v>0.6635360790730126</v>
-      </c>
-      <c r="O17">
-        <f t="shared" si="2"/>
-        <v>0.3503753231992241</v>
-      </c>
-      <c r="P17">
-        <f t="shared" si="2"/>
-        <v>-0.28264348963971025</v>
-      </c>
-      <c r="Q17">
-        <f t="shared" si="2"/>
-        <v>-0.48306751694697775</v>
-      </c>
-      <c r="R17">
-        <f t="shared" si="2"/>
-        <v>0.77849894416152299</v>
-      </c>
-      <c r="S17">
-        <f t="shared" si="2"/>
-        <v>0.73376175786203901</v>
-      </c>
-      <c r="T17">
-        <f t="shared" si="2"/>
-        <v>0.3645204210188257</v>
-      </c>
-      <c r="U17">
-        <f t="shared" si="2"/>
-        <v>-0.45428878410594931</v>
-      </c>
-    </row>
-    <row r="18" spans="1:21">
-      <c r="A18" t="s">
-        <v>40</v>
-      </c>
-      <c r="B18">
-        <v>4</v>
-      </c>
-      <c r="C18">
-        <v>40</v>
-      </c>
-      <c r="D18">
-        <v>1</v>
-      </c>
-      <c r="E18">
-        <v>10</v>
-      </c>
-      <c r="F18">
-        <v>0</v>
-      </c>
-      <c r="G18">
-        <v>0</v>
-      </c>
-      <c r="H18">
-        <v>0</v>
-      </c>
-      <c r="I18">
-        <v>0</v>
-      </c>
-      <c r="J18">
-        <v>5</v>
-      </c>
-      <c r="K18" s="2">
-        <v>50</v>
-      </c>
-      <c r="L18">
-        <f t="shared" si="3"/>
-        <v>-1.0467802484906059</v>
-      </c>
-      <c r="M18">
-        <f t="shared" si="2"/>
-        <v>0.56614734957686197</v>
-      </c>
-      <c r="N18">
-        <f t="shared" si="2"/>
-        <v>-0.99115701811531265</v>
-      </c>
-      <c r="O18">
-        <f t="shared" si="2"/>
-        <v>-0.51991176990852639</v>
-      </c>
-      <c r="P18">
-        <f t="shared" si="2"/>
-        <v>-0.92780797686078786</v>
-      </c>
-      <c r="Q18">
-        <f t="shared" si="2"/>
-        <v>-1.251584021180806</v>
-      </c>
-      <c r="R18">
-        <f t="shared" si="2"/>
-        <v>-0.97312368020190387</v>
-      </c>
-      <c r="S18">
-        <f t="shared" si="2"/>
-        <v>-1.3207711641516702</v>
-      </c>
-      <c r="T18">
-        <f t="shared" si="2"/>
-        <v>-1.0439864857979166</v>
-      </c>
-      <c r="U18">
-        <f t="shared" si="2"/>
-        <v>0.68401436243225344</v>
-      </c>
-    </row>
-    <row r="19" spans="1:21">
-      <c r="A19" t="s">
-        <v>43</v>
-      </c>
-      <c r="B19">
-        <v>13</v>
-      </c>
-      <c r="C19">
-        <v>24</v>
-      </c>
-      <c r="D19">
-        <v>24</v>
-      </c>
-      <c r="E19">
-        <v>44</v>
-      </c>
-      <c r="F19">
-        <v>2</v>
-      </c>
-      <c r="G19">
-        <v>4</v>
-      </c>
-      <c r="H19">
-        <v>2</v>
-      </c>
-      <c r="I19">
-        <v>4</v>
-      </c>
-      <c r="J19">
-        <v>13</v>
-      </c>
-      <c r="K19" s="2">
-        <v>24</v>
-      </c>
-      <c r="L19">
-        <f t="shared" si="3"/>
-        <v>-0.58127091445595991</v>
-      </c>
-      <c r="M19">
-        <f t="shared" si="2"/>
-        <v>-0.90846900280938248</v>
-      </c>
-      <c r="N19">
-        <f t="shared" si="2"/>
-        <v>1.0118925205863443</v>
-      </c>
-      <c r="O19">
-        <f t="shared" si="2"/>
-        <v>2.1700665178790661</v>
-      </c>
-      <c r="P19">
-        <f t="shared" si="2"/>
-        <v>-0.6697421819723568</v>
-      </c>
-      <c r="Q19">
-        <f t="shared" si="2"/>
-        <v>-0.63677081779374334</v>
-      </c>
-      <c r="R19">
-        <f t="shared" si="2"/>
-        <v>-0.38924947208076155</v>
-      </c>
-      <c r="S19">
-        <f t="shared" si="2"/>
-        <v>4.8917450524135916E-2</v>
-      </c>
-      <c r="T19">
-        <f t="shared" si="2"/>
-        <v>-0.55407103994861506</v>
-      </c>
-      <c r="U19">
-        <f t="shared" si="2"/>
-        <v>-0.7253133428055214</v>
-      </c>
-    </row>
-    <row r="20" spans="1:21">
-      <c r="A20" t="s">
-        <v>46</v>
-      </c>
-      <c r="B20">
-        <v>24</v>
-      </c>
-      <c r="C20">
-        <v>21</v>
-      </c>
-      <c r="D20">
-        <v>44</v>
-      </c>
-      <c r="E20">
-        <v>39</v>
-      </c>
-      <c r="F20">
-        <v>14</v>
-      </c>
-      <c r="G20">
-        <v>12</v>
-      </c>
-      <c r="H20">
-        <v>6</v>
-      </c>
-      <c r="I20">
-        <v>5</v>
-      </c>
-      <c r="J20">
-        <v>26</v>
-      </c>
-      <c r="K20" s="2">
-        <v>23</v>
-      </c>
-      <c r="L20">
-        <f t="shared" si="3"/>
-        <v>-1.2315061746948261E-2</v>
-      </c>
-      <c r="M20">
-        <f t="shared" si="2"/>
-        <v>-1.1849595688818033</v>
-      </c>
-      <c r="N20">
-        <f t="shared" si="2"/>
-        <v>2.7536747281530025</v>
-      </c>
-      <c r="O20">
-        <f t="shared" si="2"/>
-        <v>1.7744814755573612</v>
-      </c>
-      <c r="P20">
-        <f t="shared" si="2"/>
-        <v>0.87865258735822949</v>
-      </c>
-      <c r="Q20">
-        <f t="shared" si="2"/>
-        <v>0.59285558898038193</v>
-      </c>
-      <c r="R20">
-        <f t="shared" si="2"/>
-        <v>0.77849894416152299</v>
-      </c>
-      <c r="S20">
-        <f t="shared" si="2"/>
-        <v>0.39133960419308744</v>
-      </c>
-      <c r="T20">
-        <f t="shared" si="2"/>
-        <v>0.24204155955650025</v>
-      </c>
-      <c r="U20">
-        <f>STANDARDIZE(K20,K$4,K$5)</f>
-        <v>-0.77951825454543577</v>
-      </c>
-    </row>
-    <row r="21" spans="1:21">
-      <c r="A21" t="s">
-        <v>49</v>
-      </c>
-      <c r="B21">
-        <v>12</v>
-      </c>
-      <c r="C21">
-        <v>29</v>
-      </c>
-      <c r="D21">
-        <v>0</v>
-      </c>
-      <c r="E21">
-        <v>0</v>
-      </c>
-      <c r="F21">
-        <v>1</v>
-      </c>
-      <c r="G21">
-        <v>2</v>
-      </c>
-      <c r="H21">
-        <v>0</v>
-      </c>
-      <c r="I21">
-        <v>0</v>
-      </c>
-      <c r="J21">
-        <v>28</v>
-      </c>
-      <c r="K21" s="2">
-        <v>68</v>
-      </c>
-      <c r="L21">
-        <f t="shared" si="3"/>
-        <v>-0.63299417379314282</v>
-      </c>
-      <c r="M21">
-        <f t="shared" si="2"/>
-        <v>-0.44765139268868109</v>
-      </c>
-      <c r="N21">
-        <f t="shared" si="2"/>
-        <v>-1.0782461284936455</v>
-      </c>
-      <c r="O21">
-        <f t="shared" si="2"/>
-        <v>-1.311081854551936</v>
-      </c>
-      <c r="P21">
-        <f t="shared" si="2"/>
-        <v>-0.79877507941657233</v>
-      </c>
-      <c r="Q21">
-        <f t="shared" si="2"/>
-        <v>-0.94417741948727474</v>
-      </c>
-      <c r="R21">
-        <f t="shared" si="2"/>
-        <v>-0.97312368020190387</v>
-      </c>
-      <c r="S21">
-        <f t="shared" si="2"/>
-        <v>-1.3207711641516702</v>
-      </c>
-      <c r="T21">
-        <f t="shared" si="2"/>
-        <v>0.3645204210188257</v>
-      </c>
-      <c r="U21">
-        <f t="shared" si="2"/>
-        <v>1.6597027737507128</v>
-      </c>
-    </row>
-    <row r="22" spans="1:21">
-      <c r="A22" t="s">
-        <v>51</v>
-      </c>
-      <c r="B22">
-        <v>18</v>
-      </c>
-      <c r="C22">
-        <v>29</v>
-      </c>
-      <c r="D22">
-        <v>7</v>
-      </c>
-      <c r="E22">
-        <v>11</v>
-      </c>
-      <c r="F22">
-        <v>9</v>
-      </c>
-      <c r="G22">
-        <v>14</v>
-      </c>
-      <c r="H22">
-        <v>0</v>
-      </c>
-      <c r="I22">
-        <v>0</v>
-      </c>
-      <c r="J22">
-        <v>29</v>
-      </c>
-      <c r="K22" s="2">
-        <v>46</v>
-      </c>
-      <c r="L22">
-        <f t="shared" si="3"/>
-        <v>-0.32265461777004556</v>
-      </c>
-      <c r="M22">
-        <f t="shared" si="2"/>
-        <v>-0.44765139268868109</v>
-      </c>
-      <c r="N22">
-        <f t="shared" si="2"/>
-        <v>-0.4686223558453152</v>
-      </c>
-      <c r="O22">
-        <f t="shared" si="2"/>
-        <v>-0.44079476144418545</v>
-      </c>
-      <c r="P22">
-        <f t="shared" si="2"/>
-        <v>0.23348810013715188</v>
-      </c>
-      <c r="Q22">
-        <f t="shared" si="2"/>
-        <v>0.90026219067391322</v>
-      </c>
-      <c r="R22">
-        <f t="shared" si="2"/>
-        <v>-0.97312368020190387</v>
-      </c>
-      <c r="S22">
-        <f t="shared" si="2"/>
-        <v>-1.3207711641516702</v>
-      </c>
-      <c r="T22">
-        <f t="shared" si="2"/>
-        <v>0.42575985174998843</v>
-      </c>
-      <c r="U22">
-        <f t="shared" si="2"/>
-        <v>0.46719471547259578</v>
-      </c>
-    </row>
-    <row r="23" spans="1:21">
-      <c r="A23" t="s">
-        <v>55</v>
-      </c>
-      <c r="B23">
-        <v>73</v>
-      </c>
-      <c r="C23">
-        <v>38</v>
-      </c>
-      <c r="D23">
-        <v>16</v>
-      </c>
-      <c r="E23">
-        <v>8</v>
-      </c>
-      <c r="F23">
-        <v>31</v>
-      </c>
-      <c r="G23">
-        <v>16</v>
-      </c>
-      <c r="H23">
-        <v>6</v>
-      </c>
-      <c r="I23">
-        <v>3</v>
-      </c>
-      <c r="J23">
-        <v>66</v>
-      </c>
-      <c r="K23" s="2">
-        <v>34</v>
-      </c>
-      <c r="L23">
-        <f t="shared" si="3"/>
-        <v>2.5221246457750128</v>
-      </c>
-      <c r="M23">
-        <f t="shared" si="2"/>
-        <v>0.38182030552858148</v>
-      </c>
-      <c r="N23">
-        <f t="shared" si="2"/>
-        <v>0.31517963755968098</v>
-      </c>
-      <c r="O23">
-        <f t="shared" si="2"/>
-        <v>-0.67814578683720828</v>
-      </c>
-      <c r="P23">
-        <f t="shared" si="2"/>
-        <v>3.0722118439098938</v>
-      </c>
-      <c r="Q23">
-        <f t="shared" si="2"/>
-        <v>1.2076687923674445</v>
-      </c>
-      <c r="R23">
-        <f t="shared" si="2"/>
-        <v>0.77849894416152299</v>
-      </c>
-      <c r="S23">
-        <f t="shared" si="2"/>
-        <v>-0.29350470314481564</v>
-      </c>
-      <c r="T23">
-        <f t="shared" si="2"/>
-        <v>2.6916187888030088</v>
-      </c>
-      <c r="U23">
-        <f t="shared" si="2"/>
-        <v>-0.18326422540637724</v>
-      </c>
-    </row>
-    <row r="24" spans="1:21">
-      <c r="A24" t="s">
-        <v>58</v>
-      </c>
-      <c r="B24">
-        <v>5</v>
-      </c>
-      <c r="C24">
-        <v>45</v>
-      </c>
-      <c r="D24">
-        <v>0</v>
-      </c>
-      <c r="E24">
-        <v>0</v>
-      </c>
-      <c r="F24">
-        <v>0</v>
-      </c>
-      <c r="G24">
-        <v>0</v>
-      </c>
-      <c r="H24">
-        <v>0</v>
-      </c>
-      <c r="I24">
-        <v>0</v>
-      </c>
-      <c r="J24">
-        <v>6</v>
-      </c>
-      <c r="K24" s="2">
-        <v>55</v>
-      </c>
-      <c r="L24">
-        <f t="shared" si="3"/>
-        <v>-0.995056989153423</v>
-      </c>
-      <c r="M24">
-        <f t="shared" si="2"/>
-        <v>1.0269649596975634</v>
-      </c>
-      <c r="N24">
-        <f t="shared" si="2"/>
-        <v>-1.0782461284936455</v>
-      </c>
-      <c r="O24">
-        <f t="shared" si="2"/>
-        <v>-1.311081854551936</v>
-      </c>
-      <c r="P24">
-        <f t="shared" si="2"/>
-        <v>-0.92780797686078786</v>
-      </c>
-      <c r="Q24">
-        <f t="shared" si="2"/>
-        <v>-1.251584021180806</v>
-      </c>
-      <c r="R24">
-        <f t="shared" si="2"/>
-        <v>-0.97312368020190387</v>
-      </c>
-      <c r="S24">
-        <f t="shared" si="2"/>
-        <v>-1.3207711641516702</v>
-      </c>
-      <c r="T24">
-        <f t="shared" si="2"/>
-        <v>-0.98274705506675397</v>
-      </c>
-      <c r="U24">
-        <f t="shared" si="2"/>
-        <v>0.95503892113182554</v>
-      </c>
-    </row>
-    <row r="25" spans="1:21">
-      <c r="A25" t="s">
-        <v>60</v>
-      </c>
-      <c r="B25">
-        <v>21</v>
-      </c>
-      <c r="C25">
-        <v>40</v>
-      </c>
-      <c r="D25">
-        <v>5</v>
-      </c>
-      <c r="E25">
-        <v>10</v>
-      </c>
-      <c r="F25">
-        <v>8</v>
-      </c>
-      <c r="G25">
-        <v>15</v>
-      </c>
-      <c r="H25">
-        <v>1</v>
-      </c>
-      <c r="I25">
-        <v>2</v>
-      </c>
-      <c r="J25">
-        <v>17</v>
-      </c>
-      <c r="K25" s="2">
-        <v>33</v>
-      </c>
-      <c r="L25">
-        <f t="shared" si="3"/>
-        <v>-0.1674848397584969</v>
-      </c>
-      <c r="M25">
-        <f t="shared" si="2"/>
-        <v>0.56614734957686197</v>
-      </c>
-      <c r="N25">
-        <f t="shared" si="2"/>
-        <v>-0.64280057660198109</v>
-      </c>
-      <c r="O25">
-        <f t="shared" si="2"/>
-        <v>-0.51991176990852639</v>
-      </c>
-      <c r="P25">
-        <f t="shared" si="2"/>
-        <v>0.10445520269293634</v>
-      </c>
-      <c r="Q25">
-        <f t="shared" si="2"/>
-        <v>1.0539654915206789</v>
-      </c>
-      <c r="R25">
-        <f t="shared" si="2"/>
-        <v>-0.68118657614133271</v>
-      </c>
-      <c r="S25">
-        <f t="shared" si="2"/>
-        <v>-0.63592685681376715</v>
-      </c>
-      <c r="T25">
-        <f t="shared" si="2"/>
-        <v>-0.30911331702396416</v>
-      </c>
-      <c r="U25">
-        <f t="shared" si="2"/>
-        <v>-0.23746913714629164</v>
-      </c>
-    </row>
-    <row r="26" spans="1:21">
-      <c r="A26" t="s">
-        <v>62</v>
-      </c>
-      <c r="B26">
-        <v>16</v>
-      </c>
-      <c r="C26">
-        <v>43</v>
-      </c>
-      <c r="D26">
-        <v>2</v>
-      </c>
-      <c r="E26">
-        <v>5</v>
-      </c>
-      <c r="F26">
-        <v>4</v>
-      </c>
-      <c r="G26">
-        <v>11</v>
-      </c>
-      <c r="H26">
-        <v>3</v>
-      </c>
-      <c r="I26">
-        <v>8</v>
-      </c>
-      <c r="J26">
-        <v>12</v>
-      </c>
-      <c r="K26" s="2">
-        <v>32</v>
-      </c>
-      <c r="L26">
-        <f t="shared" si="3"/>
-        <v>-0.42610113644441133</v>
-      </c>
-      <c r="M26">
-        <f t="shared" ref="M26:M30" si="4">STANDARDIZE(C26,C$4,C$5)</f>
-        <v>0.84263791564928292</v>
-      </c>
-      <c r="N26">
-        <f t="shared" ref="N26:N30" si="5">STANDARDIZE(D26,D$4,D$5)</f>
-        <v>-0.90406790773697976</v>
-      </c>
-      <c r="O26">
-        <f t="shared" ref="O26:O30" si="6">STANDARDIZE(E26,E$4,E$5)</f>
-        <v>-0.91549681223023116</v>
-      </c>
-      <c r="P26">
-        <f t="shared" ref="P26:P30" si="7">STANDARDIZE(F26,F$4,F$5)</f>
-        <v>-0.41167638708392573</v>
-      </c>
-      <c r="Q26">
-        <f t="shared" ref="Q26:Q30" si="8">STANDARDIZE(G26,G$4,G$5)</f>
-        <v>0.43915228813361629</v>
-      </c>
-      <c r="R26">
-        <f t="shared" ref="R26:R30" si="9">STANDARDIZE(H26,H$4,H$5)</f>
-        <v>-9.7312368020190429E-2</v>
-      </c>
-      <c r="S26">
-        <f t="shared" ref="S26:S30" si="10">STANDARDIZE(I26,I$4,I$5)</f>
-        <v>1.4186060651999419</v>
-      </c>
-      <c r="T26">
-        <f t="shared" ref="T26:T30" si="11">STANDARDIZE(J26,J$4,J$5)</f>
-        <v>-0.61531047067977773</v>
-      </c>
-      <c r="U26">
-        <f t="shared" ref="U26:U30" si="12">STANDARDIZE(K26,K$4,K$5)</f>
-        <v>-0.29167404888620607</v>
-      </c>
-    </row>
-    <row r="27" spans="1:21">
-      <c r="A27" t="s">
-        <v>66</v>
-      </c>
-      <c r="B27">
-        <v>16</v>
-      </c>
-      <c r="C27">
-        <v>27</v>
-      </c>
-      <c r="D27">
-        <v>10</v>
-      </c>
-      <c r="E27">
-        <v>17</v>
-      </c>
-      <c r="F27">
-        <v>15</v>
-      </c>
-      <c r="G27">
-        <v>25</v>
-      </c>
-      <c r="H27">
-        <v>3</v>
-      </c>
-      <c r="I27">
-        <v>5</v>
-      </c>
-      <c r="J27">
-        <v>15</v>
-      </c>
-      <c r="K27" s="2">
-        <v>25</v>
-      </c>
-      <c r="L27">
-        <f t="shared" si="3"/>
-        <v>-0.42610113644441133</v>
-      </c>
-      <c r="M27">
-        <f t="shared" si="4"/>
-        <v>-0.63197843673696164</v>
-      </c>
-      <c r="N27">
-        <f t="shared" si="5"/>
-        <v>-0.2073550247103165</v>
-      </c>
-      <c r="O27">
-        <f t="shared" si="6"/>
-        <v>3.390728934186029E-2</v>
-      </c>
-      <c r="P27">
-        <f t="shared" si="7"/>
-        <v>1.007685484802445</v>
-      </c>
-      <c r="Q27">
-        <f t="shared" si="8"/>
+      <c r="O32" s="8">
+        <f t="shared" si="9"/>
         <v>2.5909984999883355</v>
       </c>
-      <c r="R27">
-        <f t="shared" si="9"/>
-        <v>-9.7312368020190429E-2</v>
-      </c>
-      <c r="S27">
+      <c r="P32" s="8">
         <f t="shared" si="10"/>
         <v>0.39133960419308744</v>
       </c>
-      <c r="T27">
+      <c r="Q32" s="9">
         <f t="shared" si="11"/>
-        <v>-0.43159217848628961</v>
-      </c>
-      <c r="U27">
-        <f t="shared" si="12"/>
         <v>-0.67110843106560703</v>
       </c>
-    </row>
-    <row r="28" spans="1:21">
-      <c r="A28" t="s">
+      <c r="R32" s="8">
+        <f t="shared" si="2"/>
+        <v>12.643211238906746</v>
+      </c>
+      <c r="S32" s="8">
+        <f t="shared" si="3"/>
+        <v>22.704445193579353</v>
+      </c>
+      <c r="T32" s="8">
+        <f t="shared" si="4"/>
+        <v>6.2718737441995183</v>
+      </c>
+      <c r="U32" s="8">
+        <f t="shared" si="5"/>
+        <v>6.2718737441995183</v>
+      </c>
+      <c r="V32" s="8">
+        <f t="shared" si="6"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:22" s="8" customFormat="1">
+      <c r="A33" s="8">
+        <v>19</v>
+      </c>
+      <c r="B33" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="B28">
+      <c r="C33" s="8">
         <v>34</v>
       </c>
-      <c r="C28">
+      <c r="D33" s="8">
         <v>48</v>
       </c>
-      <c r="D28">
+      <c r="E33" s="8">
         <v>4</v>
       </c>
-      <c r="E28">
+      <c r="F33" s="8">
         <v>6</v>
       </c>
-      <c r="F28">
+      <c r="G33" s="8">
         <v>2</v>
       </c>
-      <c r="G28">
+      <c r="H33" s="8">
         <v>3</v>
       </c>
-      <c r="H28">
+      <c r="I33" s="8">
         <v>3</v>
       </c>
-      <c r="I28">
+      <c r="J33" s="8">
         <v>4</v>
       </c>
-      <c r="J28">
+      <c r="K33" s="8">
         <v>28</v>
       </c>
-      <c r="K28" s="2">
+      <c r="L33" s="9">
         <v>39</v>
       </c>
-      <c r="L28">
-        <f t="shared" si="3"/>
-        <v>0.50491753162488051</v>
-      </c>
-      <c r="M28">
-        <f t="shared" si="4"/>
+      <c r="M33" s="8">
+        <f t="shared" si="7"/>
         <v>1.3034555257699842</v>
       </c>
-      <c r="N28">
-        <f t="shared" si="5"/>
-        <v>-0.72988968698031398</v>
-      </c>
-      <c r="O28">
-        <f t="shared" si="6"/>
+      <c r="N33" s="8">
+        <f t="shared" si="8"/>
         <v>-0.83637980376589016</v>
       </c>
-      <c r="P28">
-        <f t="shared" si="7"/>
-        <v>-0.6697421819723568</v>
-      </c>
-      <c r="Q28">
-        <f t="shared" si="8"/>
+      <c r="O33" s="8">
+        <f t="shared" si="9"/>
         <v>-0.79047411864050909</v>
       </c>
-      <c r="R28">
-        <f t="shared" si="9"/>
-        <v>-9.7312368020190429E-2</v>
-      </c>
-      <c r="S28">
+      <c r="P33" s="8">
         <f t="shared" si="10"/>
         <v>4.8917450524135916E-2</v>
       </c>
-      <c r="T28">
+      <c r="Q33" s="9">
         <f t="shared" si="11"/>
-        <v>0.3645204210188257</v>
-      </c>
-      <c r="U28">
-        <f t="shared" si="12"/>
         <v>8.7760333293194839E-2</v>
       </c>
-    </row>
-    <row r="29" spans="1:21">
-      <c r="A29" t="s">
+      <c r="R33" s="8">
+        <f t="shared" si="2"/>
+        <v>8.5365094072920904</v>
+      </c>
+      <c r="S33" s="8">
+        <f t="shared" si="3"/>
+        <v>7.6623921188695379</v>
+      </c>
+      <c r="T33" s="8">
+        <f t="shared" si="4"/>
+        <v>2.6676159658605836</v>
+      </c>
+      <c r="U33" s="8">
+        <f t="shared" si="5"/>
+        <v>2.6676159658605836</v>
+      </c>
+      <c r="V33" s="8">
+        <f t="shared" si="6"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:22" s="6" customFormat="1">
+      <c r="A34" s="6">
+        <v>20</v>
+      </c>
+      <c r="B34" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="B29">
+      <c r="C34" s="6">
         <v>7</v>
       </c>
-      <c r="C29">
+      <c r="D34" s="6">
         <v>30</v>
       </c>
-      <c r="D29">
+      <c r="E34" s="6">
         <v>8</v>
       </c>
-      <c r="E29">
+      <c r="F34" s="6">
         <v>35</v>
       </c>
-      <c r="F29">
+      <c r="G34" s="6">
         <v>1</v>
       </c>
-      <c r="G29">
+      <c r="H34" s="6">
         <v>4</v>
       </c>
-      <c r="H29">
+      <c r="I34" s="6">
         <v>1</v>
       </c>
-      <c r="I29">
+      <c r="J34" s="6">
         <v>4</v>
       </c>
-      <c r="J29">
+      <c r="K34" s="6">
         <v>6</v>
       </c>
-      <c r="K29" s="2">
+      <c r="L34" s="7">
         <v>26</v>
       </c>
-      <c r="L29">
-        <f t="shared" si="3"/>
-        <v>-0.89161047047905728</v>
-      </c>
-      <c r="M29">
-        <f t="shared" si="4"/>
+      <c r="M34" s="6">
+        <f t="shared" si="7"/>
         <v>-0.35548787066454079</v>
       </c>
-      <c r="N29">
-        <f t="shared" si="5"/>
-        <v>-0.38153324546698231</v>
-      </c>
-      <c r="O29">
-        <f t="shared" si="6"/>
+      <c r="N34" s="6">
+        <f t="shared" si="8"/>
         <v>1.4580134416999975</v>
       </c>
-      <c r="P29">
-        <f t="shared" si="7"/>
-        <v>-0.79877507941657233</v>
-      </c>
-      <c r="Q29">
-        <f t="shared" si="8"/>
+      <c r="O34" s="6">
+        <f t="shared" si="9"/>
         <v>-0.63677081779374334</v>
       </c>
-      <c r="R29">
-        <f t="shared" si="9"/>
-        <v>-0.68118657614133271</v>
-      </c>
-      <c r="S29">
+      <c r="P34" s="6">
         <f t="shared" si="10"/>
         <v>4.8917450524135916E-2</v>
       </c>
-      <c r="T29">
+      <c r="Q34" s="7">
         <f t="shared" si="11"/>
-        <v>-0.98274705506675397</v>
-      </c>
-      <c r="U29">
-        <f t="shared" si="12"/>
         <v>-0.61690351932569254</v>
       </c>
-    </row>
-    <row r="30" spans="1:21">
-      <c r="A30" t="s">
+      <c r="R34" s="6">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="S34" s="6">
+        <f t="shared" si="3"/>
+        <v>14.829864808128864</v>
+      </c>
+      <c r="T34" s="6">
+        <f t="shared" si="4"/>
+        <v>5.2273277495191302</v>
+      </c>
+      <c r="U34" s="6">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="V34" s="6">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:22" s="6" customFormat="1">
+      <c r="A35" s="6">
+        <v>21</v>
+      </c>
+      <c r="B35" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="B30">
+      <c r="C35" s="6">
         <v>18</v>
       </c>
-      <c r="C30">
+      <c r="D35" s="6">
         <v>31</v>
       </c>
-      <c r="D30">
+      <c r="E35" s="6">
         <v>17</v>
       </c>
-      <c r="E30">
+      <c r="F35" s="6">
         <v>29</v>
       </c>
-      <c r="F30">
+      <c r="G35" s="6">
         <v>7</v>
       </c>
-      <c r="G30">
+      <c r="H35" s="6">
         <v>12</v>
       </c>
-      <c r="H30">
+      <c r="I35" s="6">
         <v>2</v>
       </c>
-      <c r="I30">
+      <c r="J35" s="6">
         <v>3</v>
       </c>
-      <c r="J30">
+      <c r="K35" s="6">
         <v>14</v>
       </c>
-      <c r="K30" s="2">
+      <c r="L35" s="7">
         <v>24</v>
       </c>
-      <c r="L30">
-        <f t="shared" si="3"/>
-        <v>-0.32265461777004556</v>
-      </c>
-      <c r="M30">
-        <f t="shared" si="4"/>
+      <c r="M35" s="6">
+        <f t="shared" si="7"/>
         <v>-0.26332434864040055</v>
       </c>
-      <c r="N30">
-        <f t="shared" si="5"/>
-        <v>0.40226874793801387</v>
-      </c>
-      <c r="O30">
-        <f t="shared" si="6"/>
+      <c r="N35" s="6">
+        <f t="shared" si="8"/>
         <v>0.9833113909139517</v>
       </c>
-      <c r="P30">
-        <f t="shared" si="7"/>
-        <v>-2.4577694751279175E-2</v>
-      </c>
-      <c r="Q30">
-        <f t="shared" si="8"/>
+      <c r="O35" s="6">
+        <f t="shared" si="9"/>
         <v>0.59285558898038193</v>
       </c>
-      <c r="R30">
-        <f t="shared" si="9"/>
-        <v>-0.38924947208076155</v>
-      </c>
-      <c r="S30">
+      <c r="P35" s="6">
         <f t="shared" si="10"/>
         <v>-0.29350470314481564</v>
       </c>
-      <c r="T30">
+      <c r="Q35" s="7">
         <f t="shared" si="11"/>
-        <v>-0.49283160921745228</v>
-      </c>
-      <c r="U30">
-        <f t="shared" si="12"/>
         <v>-0.7253133428055214</v>
       </c>
+      <c r="R35" s="6">
+        <f t="shared" si="2"/>
+        <v>1.8748228731988286</v>
+      </c>
+      <c r="S35" s="6">
+        <f t="shared" si="3"/>
+        <v>14.404265551268731</v>
+      </c>
+      <c r="T35" s="6">
+        <f t="shared" si="4"/>
+        <v>2.9270624417643454</v>
+      </c>
+      <c r="U35" s="6">
+        <f t="shared" si="5"/>
+        <v>1.8748228731988286</v>
+      </c>
+      <c r="V35" s="6">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="V15:V35">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="num" val="1"/>
+        <cfvo type="num" val="2"/>
+        <cfvo type="num" val="3"/>
+        <color theme="8"/>
+        <color theme="9"/>
+        <color rgb="FFFFEF9C"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:F28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4879,7 +5256,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:G28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5391,7 +5768,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:F28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5837,7 +6214,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:F26"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>